<commit_message>
Membedakan jenis `Pelanggan` menjadi *corporate* dan *outsider* (personal) dimana harga `Work` untuk kedua jenis `Pelanggan` tersebut berbeda.
</commit_message>
<xml_diff>
--- a/data_awal.xlsx
+++ b/data_awal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="hibernate_sequences" sheetId="2" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="itempakaian" sheetId="1" r:id="rId3"/>
     <sheet name="kategori" sheetId="4" r:id="rId4"/>
     <sheet name="jeniswork" sheetId="5" r:id="rId5"/>
+    <sheet name="pelanggan" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="93">
   <si>
     <t>id</t>
   </si>
@@ -194,9 +195,6 @@
     <t>ItemPakaian</t>
   </si>
   <si>
-    <t>harga</t>
-  </si>
-  <si>
     <t>itemPakaian_id</t>
   </si>
   <si>
@@ -231,6 +229,75 @@
   </si>
   <si>
     <t>jeniswork</t>
+  </si>
+  <si>
+    <t>hargaCorporate</t>
+  </si>
+  <si>
+    <t>hargaOutsider</t>
+  </si>
+  <si>
+    <t>alamat</t>
+  </si>
+  <si>
+    <t>nomorTelepon</t>
+  </si>
+  <si>
+    <t>Jl. Imam Bonjol</t>
+  </si>
+  <si>
+    <t>Steven</t>
+  </si>
+  <si>
+    <t>Jl. Setia Budi</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Jl. Siantan</t>
+  </si>
+  <si>
+    <t>Bram</t>
+  </si>
+  <si>
+    <t>Jl. Sungai Raya Dalam</t>
+  </si>
+  <si>
+    <t>Edi Yi Wei</t>
+  </si>
+  <si>
+    <t>Jl. Purnama</t>
+  </si>
+  <si>
+    <t>Sandi Kosasi</t>
+  </si>
+  <si>
+    <t>Jl. Pahlawan</t>
+  </si>
+  <si>
+    <t>Yip Man</t>
+  </si>
+  <si>
+    <t>Jl. Tenaga Baru</t>
+  </si>
+  <si>
+    <t>Bruce Lee</t>
+  </si>
+  <si>
+    <t>corporate</t>
+  </si>
+  <si>
+    <t>Jl. Merdeka</t>
+  </si>
+  <si>
+    <t>PT. ABC</t>
+  </si>
+  <si>
+    <t>Jl. Teuku Umar</t>
+  </si>
+  <si>
+    <t>PT. SMIK</t>
   </si>
 </sst>
 </file>
@@ -574,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,7 +669,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -610,7 +677,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -618,7 +685,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -631,10 +698,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G145"/>
+  <dimension ref="A1:H145"/>
   <sheetViews>
-    <sheetView topLeftCell="A122" workbookViewId="0">
-      <selection sqref="A1:G145"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection sqref="A1:H145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,13 +709,13 @@
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -659,19 +726,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>59</v>
       </c>
-      <c r="G1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -684,14 +754,17 @@
       <c r="D2" s="2">
         <v>0</v>
       </c>
-      <c r="F2">
-        <v>1</v>
+      <c r="E2" s="2">
+        <v>0</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -704,14 +777,17 @@
       <c r="D3" s="2">
         <v>0</v>
       </c>
-      <c r="F3">
-        <v>2</v>
+      <c r="E3" s="2">
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -724,14 +800,18 @@
       <c r="D4" s="2">
         <v>20500</v>
       </c>
-      <c r="F4">
-        <v>3</v>
+      <c r="E4" s="2">
+        <f>ROUND(D4+5%*D4,0)</f>
+        <v>21525</v>
       </c>
       <c r="G4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -744,14 +824,18 @@
       <c r="D5" s="2">
         <v>11000</v>
       </c>
-      <c r="F5">
+      <c r="E5" s="2">
+        <f t="shared" ref="E5:E68" si="0">ROUND(D5+5%*D5,0)</f>
+        <v>11550</v>
+      </c>
+      <c r="G5">
         <v>4</v>
       </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -764,14 +848,18 @@
       <c r="D6" s="2">
         <v>12000</v>
       </c>
-      <c r="F6">
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>12600</v>
+      </c>
+      <c r="G6">
         <v>5</v>
       </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -784,14 +872,18 @@
       <c r="D7" s="2">
         <v>11000</v>
       </c>
-      <c r="F7">
-        <v>6</v>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>11550</v>
       </c>
       <c r="G7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -804,14 +896,18 @@
       <c r="D8" s="2">
         <v>11750</v>
       </c>
-      <c r="F8">
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>12338</v>
+      </c>
+      <c r="G8">
         <v>7</v>
       </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -824,14 +920,18 @@
       <c r="D9" s="2">
         <v>11500</v>
       </c>
-      <c r="F9">
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>12075</v>
+      </c>
+      <c r="G9">
         <v>8</v>
       </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -844,14 +944,18 @@
       <c r="D10" s="2">
         <v>11500</v>
       </c>
-      <c r="F10">
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>12075</v>
+      </c>
+      <c r="G10">
         <v>9</v>
       </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -864,14 +968,18 @@
       <c r="D11" s="2">
         <v>7500</v>
       </c>
-      <c r="F11">
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>7875</v>
+      </c>
+      <c r="G11">
         <v>10</v>
       </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -884,14 +992,18 @@
       <c r="D12" s="2">
         <v>7500</v>
       </c>
-      <c r="F12">
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>7875</v>
+      </c>
+      <c r="G12">
         <v>11</v>
       </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -904,14 +1016,18 @@
       <c r="D13" s="2">
         <v>6000</v>
       </c>
-      <c r="F13">
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>6300</v>
+      </c>
+      <c r="G13">
         <v>12</v>
       </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -924,14 +1040,18 @@
       <c r="D14" s="2">
         <v>16000</v>
       </c>
-      <c r="F14">
+      <c r="E14" s="2">
+        <f t="shared" si="0"/>
+        <v>16800</v>
+      </c>
+      <c r="G14">
         <v>13</v>
       </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -944,14 +1064,18 @@
       <c r="D15" s="2">
         <v>2500</v>
       </c>
-      <c r="F15">
+      <c r="E15" s="2">
+        <f t="shared" si="0"/>
+        <v>2625</v>
+      </c>
+      <c r="G15">
         <v>14</v>
       </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -964,14 +1088,18 @@
       <c r="D16" s="2">
         <v>15000</v>
       </c>
-      <c r="F16">
+      <c r="E16" s="2">
+        <f t="shared" si="0"/>
+        <v>15750</v>
+      </c>
+      <c r="G16">
         <v>15</v>
       </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -984,14 +1112,18 @@
       <c r="D17" s="2">
         <v>12500</v>
       </c>
-      <c r="F17">
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>13125</v>
+      </c>
+      <c r="G17">
         <v>16</v>
       </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1004,14 +1136,18 @@
       <c r="D18" s="2">
         <v>5500</v>
       </c>
-      <c r="F18">
+      <c r="E18" s="2">
+        <f t="shared" si="0"/>
+        <v>5775</v>
+      </c>
+      <c r="G18">
         <v>17</v>
       </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1024,14 +1160,18 @@
       <c r="D19" s="2">
         <v>20500</v>
       </c>
-      <c r="F19">
+      <c r="E19" s="2">
+        <f t="shared" si="0"/>
+        <v>21525</v>
+      </c>
+      <c r="G19">
         <v>18</v>
       </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1044,14 +1184,18 @@
       <c r="D20" s="2">
         <v>16000</v>
       </c>
-      <c r="F20">
+      <c r="E20" s="2">
+        <f t="shared" si="0"/>
+        <v>16800</v>
+      </c>
+      <c r="G20">
         <v>19</v>
       </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1064,14 +1208,18 @@
       <c r="D21" s="2">
         <v>12500</v>
       </c>
-      <c r="F21">
+      <c r="E21" s="2">
+        <f t="shared" si="0"/>
+        <v>13125</v>
+      </c>
+      <c r="G21">
         <v>20</v>
       </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1084,14 +1232,18 @@
       <c r="D22" s="2">
         <v>16500</v>
       </c>
-      <c r="F22">
+      <c r="E22" s="2">
+        <f t="shared" si="0"/>
+        <v>17325</v>
+      </c>
+      <c r="G22">
         <v>21</v>
       </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1104,14 +1256,18 @@
       <c r="D23" s="2">
         <v>26000</v>
       </c>
-      <c r="F23">
+      <c r="E23" s="2">
+        <f t="shared" si="0"/>
+        <v>27300</v>
+      </c>
+      <c r="G23">
         <v>22</v>
       </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1124,14 +1280,18 @@
       <c r="D24" s="2">
         <v>24000</v>
       </c>
-      <c r="F24">
+      <c r="E24" s="2">
+        <f t="shared" si="0"/>
+        <v>25200</v>
+      </c>
+      <c r="G24">
         <v>23</v>
       </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1144,14 +1304,18 @@
       <c r="D25" s="2">
         <v>31500</v>
       </c>
-      <c r="F25">
+      <c r="E25" s="2">
+        <f t="shared" si="0"/>
+        <v>33075</v>
+      </c>
+      <c r="G25">
         <v>24</v>
       </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1164,14 +1328,18 @@
       <c r="D26" s="2">
         <v>41500</v>
       </c>
-      <c r="F26">
+      <c r="E26" s="2">
+        <f t="shared" si="0"/>
+        <v>43575</v>
+      </c>
+      <c r="G26">
         <v>25</v>
       </c>
-      <c r="G26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1184,14 +1352,18 @@
       <c r="D27" s="2">
         <v>17500</v>
       </c>
-      <c r="F27">
+      <c r="E27" s="2">
+        <f t="shared" si="0"/>
+        <v>18375</v>
+      </c>
+      <c r="G27">
         <v>26</v>
       </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1204,14 +1376,18 @@
       <c r="D28" s="2">
         <v>28500</v>
       </c>
-      <c r="F28">
+      <c r="E28" s="2">
+        <f t="shared" si="0"/>
+        <v>29925</v>
+      </c>
+      <c r="G28">
         <v>27</v>
       </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1224,14 +1400,18 @@
       <c r="D29" s="2">
         <v>7000</v>
       </c>
-      <c r="F29">
+      <c r="E29" s="2">
+        <f t="shared" si="0"/>
+        <v>7350</v>
+      </c>
+      <c r="G29">
         <v>28</v>
       </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1244,14 +1424,18 @@
       <c r="D30" s="2">
         <v>13500</v>
       </c>
-      <c r="F30">
+      <c r="E30" s="2">
+        <f t="shared" si="0"/>
+        <v>14175</v>
+      </c>
+      <c r="G30">
         <v>29</v>
       </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1264,14 +1448,18 @@
       <c r="D31" s="2">
         <v>6500</v>
       </c>
-      <c r="F31">
+      <c r="E31" s="2">
+        <f t="shared" si="0"/>
+        <v>6825</v>
+      </c>
+      <c r="G31">
         <v>30</v>
       </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1284,14 +1472,18 @@
       <c r="D32" s="2">
         <v>4300</v>
       </c>
-      <c r="F32">
+      <c r="E32" s="2">
+        <f t="shared" si="0"/>
+        <v>4515</v>
+      </c>
+      <c r="G32">
         <v>31</v>
       </c>
-      <c r="G32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1304,14 +1496,18 @@
       <c r="D33" s="2">
         <v>2500</v>
       </c>
-      <c r="F33">
+      <c r="E33" s="2">
+        <f t="shared" si="0"/>
+        <v>2625</v>
+      </c>
+      <c r="G33">
         <v>32</v>
       </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1324,14 +1520,18 @@
       <c r="D34" s="2">
         <v>2000</v>
       </c>
-      <c r="F34">
+      <c r="E34" s="2">
+        <f t="shared" si="0"/>
+        <v>2100</v>
+      </c>
+      <c r="G34">
         <v>33</v>
       </c>
-      <c r="G34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1344,14 +1544,18 @@
       <c r="D35" s="2">
         <v>3500</v>
       </c>
-      <c r="F35">
+      <c r="E35" s="2">
+        <f t="shared" si="0"/>
+        <v>3675</v>
+      </c>
+      <c r="G35">
         <v>34</v>
       </c>
-      <c r="G35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1364,14 +1568,18 @@
       <c r="D36" s="2">
         <v>4500</v>
       </c>
-      <c r="F36">
+      <c r="E36" s="2">
+        <f t="shared" si="0"/>
+        <v>4725</v>
+      </c>
+      <c r="G36">
         <v>35</v>
       </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1384,14 +1592,18 @@
       <c r="D37" s="2">
         <v>2500</v>
       </c>
-      <c r="F37">
+      <c r="E37" s="2">
+        <f t="shared" si="0"/>
+        <v>2625</v>
+      </c>
+      <c r="G37">
         <v>36</v>
       </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1404,14 +1616,18 @@
       <c r="D38" s="2">
         <v>7000</v>
       </c>
-      <c r="F38">
+      <c r="E38" s="2">
+        <f t="shared" si="0"/>
+        <v>7350</v>
+      </c>
+      <c r="G38">
         <v>37</v>
       </c>
-      <c r="G38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1424,14 +1640,18 @@
       <c r="D39" s="2">
         <v>10500</v>
       </c>
-      <c r="F39">
+      <c r="E39" s="2">
+        <f t="shared" si="0"/>
+        <v>11025</v>
+      </c>
+      <c r="G39">
         <v>38</v>
       </c>
-      <c r="G39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1444,14 +1664,18 @@
       <c r="D40" s="2">
         <v>3500</v>
       </c>
-      <c r="F40">
+      <c r="E40" s="2">
+        <f t="shared" si="0"/>
+        <v>3675</v>
+      </c>
+      <c r="G40">
         <v>39</v>
       </c>
-      <c r="G40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1464,14 +1688,18 @@
       <c r="D41" s="2">
         <v>3000</v>
       </c>
-      <c r="F41">
+      <c r="E41" s="2">
+        <f t="shared" si="0"/>
+        <v>3150</v>
+      </c>
+      <c r="G41">
         <v>40</v>
       </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1484,14 +1712,18 @@
       <c r="D42" s="2">
         <v>2500</v>
       </c>
-      <c r="F42">
+      <c r="E42" s="2">
+        <f t="shared" si="0"/>
+        <v>2625</v>
+      </c>
+      <c r="G42">
         <v>41</v>
       </c>
-      <c r="G42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1504,14 +1736,18 @@
       <c r="D43" s="2">
         <v>4500</v>
       </c>
-      <c r="F43">
+      <c r="E43" s="2">
+        <f t="shared" si="0"/>
+        <v>4725</v>
+      </c>
+      <c r="G43">
         <v>42</v>
       </c>
-      <c r="G43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1524,14 +1760,18 @@
       <c r="D44" s="2">
         <v>4000</v>
       </c>
-      <c r="F44">
+      <c r="E44" s="2">
+        <f t="shared" si="0"/>
+        <v>4200</v>
+      </c>
+      <c r="G44">
         <v>43</v>
       </c>
-      <c r="G44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1544,14 +1784,18 @@
       <c r="D45" s="2">
         <v>3500</v>
       </c>
-      <c r="F45">
+      <c r="E45" s="2">
+        <f t="shared" si="0"/>
+        <v>3675</v>
+      </c>
+      <c r="G45">
         <v>44</v>
       </c>
-      <c r="G45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1564,14 +1808,18 @@
       <c r="D46" s="2">
         <v>6000</v>
       </c>
-      <c r="F46">
+      <c r="E46" s="2">
+        <f t="shared" si="0"/>
+        <v>6300</v>
+      </c>
+      <c r="G46">
         <v>45</v>
       </c>
-      <c r="G46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1584,14 +1832,18 @@
       <c r="D47" s="2">
         <v>2000</v>
       </c>
-      <c r="F47">
+      <c r="E47" s="2">
+        <f t="shared" si="0"/>
+        <v>2100</v>
+      </c>
+      <c r="G47">
         <v>46</v>
       </c>
-      <c r="G47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1604,14 +1856,18 @@
       <c r="D48" s="2">
         <v>15000</v>
       </c>
-      <c r="F48">
+      <c r="E48" s="2">
+        <f t="shared" si="0"/>
+        <v>15750</v>
+      </c>
+      <c r="G48">
         <v>47</v>
       </c>
-      <c r="G48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1624,14 +1880,18 @@
       <c r="D49" s="2">
         <v>12500</v>
       </c>
-      <c r="F49">
+      <c r="E49" s="2">
+        <f t="shared" si="0"/>
+        <v>13125</v>
+      </c>
+      <c r="G49">
         <v>48</v>
       </c>
-      <c r="G49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1644,14 +1904,18 @@
       <c r="D50" s="2">
         <v>22500</v>
       </c>
-      <c r="F50">
-        <v>1</v>
+      <c r="E50" s="2">
+        <f t="shared" si="0"/>
+        <v>23625</v>
       </c>
       <c r="G50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="H50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1664,14 +1928,18 @@
       <c r="D51" s="2">
         <v>16000</v>
       </c>
-      <c r="F51">
-        <v>2</v>
+      <c r="E51" s="2">
+        <f t="shared" si="0"/>
+        <v>16800</v>
       </c>
       <c r="G51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1684,14 +1952,18 @@
       <c r="D52" s="2">
         <v>21500</v>
       </c>
-      <c r="F52">
-        <v>3</v>
+      <c r="E52" s="2">
+        <f t="shared" si="0"/>
+        <v>22575</v>
       </c>
       <c r="G52">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1704,14 +1976,18 @@
       <c r="D53" s="2">
         <v>12000</v>
       </c>
-      <c r="F53">
+      <c r="E53" s="2">
+        <f t="shared" si="0"/>
+        <v>12600</v>
+      </c>
+      <c r="G53">
         <v>4</v>
       </c>
-      <c r="G53">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1724,14 +2000,18 @@
       <c r="D54" s="2">
         <v>15000</v>
       </c>
-      <c r="F54">
+      <c r="E54" s="2">
+        <f t="shared" si="0"/>
+        <v>15750</v>
+      </c>
+      <c r="G54">
         <v>5</v>
       </c>
-      <c r="G54">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1744,14 +2024,18 @@
       <c r="D55" s="2">
         <v>13000</v>
       </c>
-      <c r="F55">
-        <v>6</v>
+      <c r="E55" s="2">
+        <f t="shared" si="0"/>
+        <v>13650</v>
       </c>
       <c r="G55">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="H55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1764,14 +2048,18 @@
       <c r="D56" s="2">
         <v>15500</v>
       </c>
-      <c r="F56">
+      <c r="E56" s="2">
+        <f t="shared" si="0"/>
+        <v>16275</v>
+      </c>
+      <c r="G56">
         <v>7</v>
       </c>
-      <c r="G56">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1784,14 +2072,18 @@
       <c r="D57" s="2">
         <v>15000</v>
       </c>
-      <c r="F57">
+      <c r="E57" s="2">
+        <f t="shared" si="0"/>
+        <v>15750</v>
+      </c>
+      <c r="G57">
         <v>8</v>
       </c>
-      <c r="G57">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1804,14 +2096,18 @@
       <c r="D58" s="2">
         <v>13000</v>
       </c>
-      <c r="F58">
+      <c r="E58" s="2">
+        <f t="shared" si="0"/>
+        <v>13650</v>
+      </c>
+      <c r="G58">
         <v>9</v>
       </c>
-      <c r="G58">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1824,14 +2120,18 @@
       <c r="D59" s="2">
         <v>15500</v>
       </c>
-      <c r="F59">
+      <c r="E59" s="2">
+        <f t="shared" si="0"/>
+        <v>16275</v>
+      </c>
+      <c r="G59">
         <v>10</v>
       </c>
-      <c r="G59">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1844,14 +2144,18 @@
       <c r="D60" s="2">
         <v>15000</v>
       </c>
-      <c r="F60">
+      <c r="E60" s="2">
+        <f t="shared" si="0"/>
+        <v>15750</v>
+      </c>
+      <c r="G60">
         <v>11</v>
       </c>
-      <c r="G60">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1864,14 +2168,18 @@
       <c r="D61" s="2">
         <v>13000</v>
       </c>
-      <c r="F61">
+      <c r="E61" s="2">
+        <f t="shared" si="0"/>
+        <v>13650</v>
+      </c>
+      <c r="G61">
         <v>12</v>
       </c>
-      <c r="G61">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1884,14 +2192,18 @@
       <c r="D62" s="2">
         <v>9000</v>
       </c>
-      <c r="F62">
+      <c r="E62" s="2">
+        <f t="shared" si="0"/>
+        <v>9450</v>
+      </c>
+      <c r="G62">
         <v>13</v>
       </c>
-      <c r="G62">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1904,14 +2216,18 @@
       <c r="D63" s="2">
         <v>9000</v>
       </c>
-      <c r="F63">
+      <c r="E63" s="2">
+        <f t="shared" si="0"/>
+        <v>9450</v>
+      </c>
+      <c r="G63">
         <v>14</v>
       </c>
-      <c r="G63">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1924,14 +2240,18 @@
       <c r="D64" s="2">
         <v>8000</v>
       </c>
-      <c r="F64">
+      <c r="E64" s="2">
+        <f t="shared" si="0"/>
+        <v>8400</v>
+      </c>
+      <c r="G64">
         <v>15</v>
       </c>
-      <c r="G64">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1944,14 +2264,18 @@
       <c r="D65" s="2">
         <v>0</v>
       </c>
-      <c r="F65">
+      <c r="E65" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G65">
         <v>16</v>
       </c>
-      <c r="G65">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1964,14 +2288,18 @@
       <c r="D66" s="2">
         <v>0</v>
       </c>
-      <c r="F66">
+      <c r="E66" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G66">
         <v>17</v>
       </c>
-      <c r="G66">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1984,14 +2312,18 @@
       <c r="D67" s="2">
         <v>16500</v>
       </c>
-      <c r="F67">
+      <c r="E67" s="2">
+        <f t="shared" si="0"/>
+        <v>17325</v>
+      </c>
+      <c r="G67">
         <v>18</v>
       </c>
-      <c r="G67">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2004,14 +2336,18 @@
       <c r="D68" s="2">
         <v>14500</v>
       </c>
-      <c r="F68">
+      <c r="E68" s="2">
+        <f t="shared" si="0"/>
+        <v>15225</v>
+      </c>
+      <c r="G68">
         <v>19</v>
       </c>
-      <c r="G68">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2024,14 +2360,18 @@
       <c r="D69" s="2">
         <v>7500</v>
       </c>
-      <c r="F69">
+      <c r="E69" s="2">
+        <f t="shared" ref="E69:E132" si="1">ROUND(D69+5%*D69,0)</f>
+        <v>7875</v>
+      </c>
+      <c r="G69">
         <v>20</v>
       </c>
-      <c r="G69">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2044,14 +2384,18 @@
       <c r="D70" s="2">
         <v>23500</v>
       </c>
-      <c r="F70">
+      <c r="E70" s="2">
+        <f t="shared" si="1"/>
+        <v>24675</v>
+      </c>
+      <c r="G70">
         <v>21</v>
       </c>
-      <c r="G70">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2064,14 +2408,18 @@
       <c r="D71" s="2">
         <v>19000</v>
       </c>
-      <c r="F71">
+      <c r="E71" s="2">
+        <f t="shared" si="1"/>
+        <v>19950</v>
+      </c>
+      <c r="G71">
         <v>22</v>
       </c>
-      <c r="G71">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2084,14 +2432,18 @@
       <c r="D72" s="2">
         <v>17500</v>
       </c>
-      <c r="F72">
+      <c r="E72" s="2">
+        <f t="shared" si="1"/>
+        <v>18375</v>
+      </c>
+      <c r="G72">
         <v>23</v>
       </c>
-      <c r="G72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2104,14 +2456,18 @@
       <c r="D73" s="2">
         <v>22500</v>
       </c>
-      <c r="F73">
+      <c r="E73" s="2">
+        <f t="shared" si="1"/>
+        <v>23625</v>
+      </c>
+      <c r="G73">
         <v>24</v>
       </c>
-      <c r="G73">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2124,14 +2480,18 @@
       <c r="D74" s="2">
         <v>30000</v>
       </c>
-      <c r="F74">
+      <c r="E74" s="2">
+        <f t="shared" si="1"/>
+        <v>31500</v>
+      </c>
+      <c r="G74">
         <v>25</v>
       </c>
-      <c r="G74">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2144,14 +2504,18 @@
       <c r="D75" s="2">
         <v>26000</v>
       </c>
-      <c r="F75">
+      <c r="E75" s="2">
+        <f t="shared" si="1"/>
+        <v>27300</v>
+      </c>
+      <c r="G75">
         <v>26</v>
       </c>
-      <c r="G75">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2164,14 +2528,18 @@
       <c r="D76" s="2">
         <v>35500</v>
       </c>
-      <c r="F76">
+      <c r="E76" s="2">
+        <f t="shared" si="1"/>
+        <v>37275</v>
+      </c>
+      <c r="G76">
         <v>27</v>
       </c>
-      <c r="G76">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2184,14 +2552,18 @@
       <c r="D77" s="2">
         <v>44500</v>
       </c>
-      <c r="F77">
+      <c r="E77" s="2">
+        <f t="shared" si="1"/>
+        <v>46725</v>
+      </c>
+      <c r="G77">
         <v>28</v>
       </c>
-      <c r="G77">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2204,14 +2576,18 @@
       <c r="D78" s="2">
         <v>20500</v>
       </c>
-      <c r="F78">
+      <c r="E78" s="2">
+        <f t="shared" si="1"/>
+        <v>21525</v>
+      </c>
+      <c r="G78">
         <v>29</v>
       </c>
-      <c r="G78">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2224,14 +2600,18 @@
       <c r="D79" s="2">
         <v>34500</v>
       </c>
-      <c r="F79">
+      <c r="E79" s="2">
+        <f t="shared" si="1"/>
+        <v>36225</v>
+      </c>
+      <c r="G79">
         <v>30</v>
       </c>
-      <c r="G79">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2244,14 +2624,18 @@
       <c r="D80" s="2">
         <v>9500</v>
       </c>
-      <c r="F80">
+      <c r="E80" s="2">
+        <f t="shared" si="1"/>
+        <v>9975</v>
+      </c>
+      <c r="G80">
         <v>31</v>
       </c>
-      <c r="G80">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2264,14 +2648,18 @@
       <c r="D81" s="2">
         <v>15500</v>
       </c>
-      <c r="F81">
+      <c r="E81" s="2">
+        <f t="shared" si="1"/>
+        <v>16275</v>
+      </c>
+      <c r="G81">
         <v>32</v>
       </c>
-      <c r="G81">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2284,14 +2672,18 @@
       <c r="D82" s="2">
         <v>8500</v>
       </c>
-      <c r="F82">
+      <c r="E82" s="2">
+        <f t="shared" si="1"/>
+        <v>8925</v>
+      </c>
+      <c r="G82">
         <v>33</v>
       </c>
-      <c r="G82">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2304,14 +2696,18 @@
       <c r="D83" s="2">
         <v>0</v>
       </c>
-      <c r="F83">
+      <c r="E83" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G83">
         <v>34</v>
       </c>
-      <c r="G83">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2324,14 +2720,18 @@
       <c r="D84" s="2">
         <v>0</v>
       </c>
-      <c r="F84">
+      <c r="E84" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G84">
         <v>35</v>
       </c>
-      <c r="G84">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2344,14 +2744,18 @@
       <c r="D85" s="2">
         <v>0</v>
       </c>
-      <c r="F85">
+      <c r="E85" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G85">
         <v>36</v>
       </c>
-      <c r="G85">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2364,14 +2768,18 @@
       <c r="D86" s="2">
         <v>0</v>
       </c>
-      <c r="F86">
+      <c r="E86" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G86">
         <v>37</v>
       </c>
-      <c r="G86">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2384,14 +2792,18 @@
       <c r="D87" s="2">
         <v>0</v>
       </c>
-      <c r="F87">
+      <c r="E87" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G87">
         <v>38</v>
       </c>
-      <c r="G87">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2404,14 +2816,18 @@
       <c r="D88" s="2">
         <v>0</v>
       </c>
-      <c r="F88">
+      <c r="E88" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G88">
         <v>39</v>
       </c>
-      <c r="G88">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2424,14 +2840,18 @@
       <c r="D89" s="2">
         <v>0</v>
       </c>
-      <c r="F89">
+      <c r="E89" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G89">
         <v>40</v>
       </c>
-      <c r="G89">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2444,14 +2864,18 @@
       <c r="D90" s="2">
         <v>0</v>
       </c>
-      <c r="F90">
+      <c r="E90" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G90">
         <v>41</v>
       </c>
-      <c r="G90">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2464,14 +2888,18 @@
       <c r="D91" s="2">
         <v>0</v>
       </c>
-      <c r="F91">
+      <c r="E91" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G91">
         <v>42</v>
       </c>
-      <c r="G91">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2484,14 +2912,18 @@
       <c r="D92" s="2">
         <v>0</v>
       </c>
-      <c r="F92">
+      <c r="E92" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G92">
         <v>43</v>
       </c>
-      <c r="G92">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2504,14 +2936,18 @@
       <c r="D93" s="2">
         <v>0</v>
       </c>
-      <c r="F93">
+      <c r="E93" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G93">
         <v>44</v>
       </c>
-      <c r="G93">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2524,14 +2960,18 @@
       <c r="D94" s="2">
         <v>8000</v>
       </c>
-      <c r="F94">
+      <c r="E94" s="2">
+        <f t="shared" si="1"/>
+        <v>8400</v>
+      </c>
+      <c r="G94">
         <v>45</v>
       </c>
-      <c r="G94">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H94">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2544,14 +2984,18 @@
       <c r="D95" s="2">
         <v>0</v>
       </c>
-      <c r="F95">
+      <c r="E95" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G95">
         <v>46</v>
       </c>
-      <c r="G95">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2564,14 +3008,18 @@
       <c r="D96" s="2">
         <v>0</v>
       </c>
-      <c r="F96">
+      <c r="E96" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G96">
         <v>47</v>
       </c>
-      <c r="G96">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2584,14 +3032,18 @@
       <c r="D97" s="2">
         <v>15000</v>
       </c>
-      <c r="F97">
+      <c r="E97" s="2">
+        <f t="shared" si="1"/>
+        <v>15750</v>
+      </c>
+      <c r="G97">
         <v>48</v>
       </c>
-      <c r="G97">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H97">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2604,14 +3056,18 @@
       <c r="D98" s="2">
         <v>16000</v>
       </c>
-      <c r="F98">
-        <v>1</v>
+      <c r="E98" s="2">
+        <f t="shared" si="1"/>
+        <v>16800</v>
       </c>
       <c r="G98">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="H98">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2624,14 +3080,18 @@
       <c r="D99" s="2">
         <v>11000</v>
       </c>
-      <c r="F99">
-        <v>2</v>
+      <c r="E99" s="2">
+        <f t="shared" si="1"/>
+        <v>11550</v>
       </c>
       <c r="G99">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H99">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -2644,14 +3104,18 @@
       <c r="D100" s="2">
         <v>15500</v>
       </c>
-      <c r="F100">
-        <v>3</v>
+      <c r="E100" s="2">
+        <f t="shared" si="1"/>
+        <v>16275</v>
       </c>
       <c r="G100">
         <v>3</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H100">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -2664,14 +3128,18 @@
       <c r="D101" s="2">
         <v>7500</v>
       </c>
-      <c r="F101">
+      <c r="E101" s="2">
+        <f t="shared" si="1"/>
+        <v>7875</v>
+      </c>
+      <c r="G101">
         <v>4</v>
       </c>
-      <c r="G101">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H101">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -2684,14 +3152,18 @@
       <c r="D102" s="2">
         <v>8500</v>
       </c>
-      <c r="F102">
+      <c r="E102" s="2">
+        <f t="shared" si="1"/>
+        <v>8925</v>
+      </c>
+      <c r="G102">
         <v>5</v>
       </c>
-      <c r="G102">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H102">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -2704,14 +3176,18 @@
       <c r="D103" s="2">
         <v>7000</v>
       </c>
-      <c r="F103">
-        <v>6</v>
+      <c r="E103" s="2">
+        <f t="shared" si="1"/>
+        <v>7350</v>
       </c>
       <c r="G103">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="H103">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -2724,14 +3200,18 @@
       <c r="D104" s="2">
         <v>9500</v>
       </c>
-      <c r="F104">
+      <c r="E104" s="2">
+        <f t="shared" si="1"/>
+        <v>9975</v>
+      </c>
+      <c r="G104">
         <v>7</v>
       </c>
-      <c r="G104">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H104">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -2744,14 +3224,18 @@
       <c r="D105" s="2">
         <v>8500</v>
       </c>
-      <c r="F105">
+      <c r="E105" s="2">
+        <f t="shared" si="1"/>
+        <v>8925</v>
+      </c>
+      <c r="G105">
         <v>8</v>
       </c>
-      <c r="G105">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H105">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -2764,14 +3248,18 @@
       <c r="D106" s="2">
         <v>7000</v>
       </c>
-      <c r="F106">
+      <c r="E106" s="2">
+        <f t="shared" si="1"/>
+        <v>7350</v>
+      </c>
+      <c r="G106">
         <v>9</v>
       </c>
-      <c r="G106">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H106">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -2784,14 +3272,18 @@
       <c r="D107" s="2">
         <v>5000</v>
       </c>
-      <c r="F107">
+      <c r="E107" s="2">
+        <f t="shared" si="1"/>
+        <v>5250</v>
+      </c>
+      <c r="G107">
         <v>10</v>
       </c>
-      <c r="G107">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H107">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -2804,14 +3296,18 @@
       <c r="D108" s="2">
         <v>6000</v>
       </c>
-      <c r="F108">
+      <c r="E108" s="2">
+        <f t="shared" si="1"/>
+        <v>6300</v>
+      </c>
+      <c r="G108">
         <v>11</v>
       </c>
-      <c r="G108">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H108">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -2824,14 +3320,18 @@
       <c r="D109" s="2">
         <v>3050</v>
       </c>
-      <c r="F109">
+      <c r="E109" s="2">
+        <f t="shared" si="1"/>
+        <v>3203</v>
+      </c>
+      <c r="G109">
         <v>12</v>
       </c>
-      <c r="G109">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H109">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -2844,14 +3344,18 @@
       <c r="D110" s="2">
         <v>11000</v>
       </c>
-      <c r="F110">
+      <c r="E110" s="2">
+        <f t="shared" si="1"/>
+        <v>11550</v>
+      </c>
+      <c r="G110">
         <v>13</v>
       </c>
-      <c r="G110">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H110">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -2864,14 +3368,18 @@
       <c r="D111" s="2">
         <v>2000</v>
       </c>
-      <c r="F111">
+      <c r="E111" s="2">
+        <f t="shared" si="1"/>
+        <v>2100</v>
+      </c>
+      <c r="G111">
         <v>14</v>
       </c>
-      <c r="G111">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H111">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -2884,14 +3392,18 @@
       <c r="D112" s="2">
         <v>10500</v>
       </c>
-      <c r="F112">
+      <c r="E112" s="2">
+        <f t="shared" si="1"/>
+        <v>11025</v>
+      </c>
+      <c r="G112">
         <v>15</v>
       </c>
-      <c r="G112">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -2904,14 +3416,18 @@
       <c r="D113" s="2">
         <v>6500</v>
       </c>
-      <c r="F113">
+      <c r="E113" s="2">
+        <f t="shared" si="1"/>
+        <v>6825</v>
+      </c>
+      <c r="G113">
         <v>16</v>
       </c>
-      <c r="G113">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H113">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -2924,14 +3440,18 @@
       <c r="D114" s="2">
         <v>4500</v>
       </c>
-      <c r="F114">
+      <c r="E114" s="2">
+        <f t="shared" si="1"/>
+        <v>4725</v>
+      </c>
+      <c r="G114">
         <v>17</v>
       </c>
-      <c r="G114">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H114">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -2944,14 +3464,18 @@
       <c r="D115" s="2">
         <v>15500</v>
       </c>
-      <c r="F115">
+      <c r="E115" s="2">
+        <f t="shared" si="1"/>
+        <v>16275</v>
+      </c>
+      <c r="G115">
         <v>18</v>
       </c>
-      <c r="G115">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H115">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -2964,14 +3488,18 @@
       <c r="D116" s="2">
         <v>9500</v>
       </c>
-      <c r="F116">
+      <c r="E116" s="2">
+        <f t="shared" si="1"/>
+        <v>9975</v>
+      </c>
+      <c r="G116">
         <v>19</v>
       </c>
-      <c r="G116">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H116">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -2984,14 +3512,18 @@
       <c r="D117" s="2">
         <v>9500</v>
       </c>
-      <c r="F117">
+      <c r="E117" s="2">
+        <f t="shared" si="1"/>
+        <v>9975</v>
+      </c>
+      <c r="G117">
         <v>20</v>
       </c>
-      <c r="G117">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H117">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -3004,14 +3536,18 @@
       <c r="D118" s="2">
         <v>12500</v>
       </c>
-      <c r="F118">
+      <c r="E118" s="2">
+        <f t="shared" si="1"/>
+        <v>13125</v>
+      </c>
+      <c r="G118">
         <v>21</v>
       </c>
-      <c r="G118">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H118">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -3024,14 +3560,18 @@
       <c r="D119" s="2">
         <v>21000</v>
       </c>
-      <c r="F119">
+      <c r="E119" s="2">
+        <f t="shared" si="1"/>
+        <v>22050</v>
+      </c>
+      <c r="G119">
         <v>22</v>
       </c>
-      <c r="G119">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H119">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -3044,14 +3584,18 @@
       <c r="D120" s="2">
         <v>19000</v>
       </c>
-      <c r="F120">
+      <c r="E120" s="2">
+        <f t="shared" si="1"/>
+        <v>19950</v>
+      </c>
+      <c r="G120">
         <v>23</v>
       </c>
-      <c r="G120">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H120">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -3064,14 +3608,18 @@
       <c r="D121" s="2">
         <v>29500</v>
       </c>
-      <c r="F121">
+      <c r="E121" s="2">
+        <f t="shared" si="1"/>
+        <v>30975</v>
+      </c>
+      <c r="G121">
         <v>24</v>
       </c>
-      <c r="G121">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H121">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -3084,14 +3632,18 @@
       <c r="D122" s="2">
         <v>39500</v>
       </c>
-      <c r="F122">
+      <c r="E122" s="2">
+        <f t="shared" si="1"/>
+        <v>41475</v>
+      </c>
+      <c r="G122">
         <v>25</v>
       </c>
-      <c r="G122">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H122">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -3104,14 +3656,18 @@
       <c r="D123" s="2">
         <v>12500</v>
       </c>
-      <c r="F123">
+      <c r="E123" s="2">
+        <f t="shared" si="1"/>
+        <v>13125</v>
+      </c>
+      <c r="G123">
         <v>26</v>
       </c>
-      <c r="G123">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H123">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -3124,14 +3680,18 @@
       <c r="D124" s="2">
         <v>20500</v>
       </c>
-      <c r="F124">
+      <c r="E124" s="2">
+        <f t="shared" si="1"/>
+        <v>21525</v>
+      </c>
+      <c r="G124">
         <v>27</v>
       </c>
-      <c r="G124">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H124">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -3144,14 +3704,18 @@
       <c r="D125" s="2">
         <v>5500</v>
       </c>
-      <c r="F125">
+      <c r="E125" s="2">
+        <f t="shared" si="1"/>
+        <v>5775</v>
+      </c>
+      <c r="G125">
         <v>28</v>
       </c>
-      <c r="G125">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H125">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -3164,14 +3728,18 @@
       <c r="D126" s="2">
         <v>6500</v>
       </c>
-      <c r="F126">
+      <c r="E126" s="2">
+        <f t="shared" si="1"/>
+        <v>6825</v>
+      </c>
+      <c r="G126">
         <v>29</v>
       </c>
-      <c r="G126">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H126">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -3184,14 +3752,18 @@
       <c r="D127" s="2">
         <v>4000</v>
       </c>
-      <c r="F127">
+      <c r="E127" s="2">
+        <f t="shared" si="1"/>
+        <v>4200</v>
+      </c>
+      <c r="G127">
         <v>30</v>
       </c>
-      <c r="G127">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H127">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -3204,14 +3776,18 @@
       <c r="D128" s="2">
         <v>3000</v>
       </c>
-      <c r="F128">
+      <c r="E128" s="2">
+        <f t="shared" si="1"/>
+        <v>3150</v>
+      </c>
+      <c r="G128">
         <v>31</v>
       </c>
-      <c r="G128">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H128">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -3224,14 +3800,18 @@
       <c r="D129" s="2">
         <v>2000</v>
       </c>
-      <c r="F129">
+      <c r="E129" s="2">
+        <f t="shared" si="1"/>
+        <v>2100</v>
+      </c>
+      <c r="G129">
         <v>32</v>
       </c>
-      <c r="G129">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H129">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
@@ -3244,14 +3824,18 @@
       <c r="D130" s="2">
         <v>1500</v>
       </c>
-      <c r="F130">
+      <c r="E130" s="2">
+        <f t="shared" si="1"/>
+        <v>1575</v>
+      </c>
+      <c r="G130">
         <v>33</v>
       </c>
-      <c r="G130">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H130">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
@@ -3264,14 +3848,18 @@
       <c r="D131" s="2">
         <v>2000</v>
       </c>
-      <c r="F131">
+      <c r="E131" s="2">
+        <f t="shared" si="1"/>
+        <v>2100</v>
+      </c>
+      <c r="G131">
         <v>34</v>
       </c>
-      <c r="G131">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H131">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
@@ -3284,14 +3872,18 @@
       <c r="D132" s="2">
         <v>3000</v>
       </c>
-      <c r="F132">
+      <c r="E132" s="2">
+        <f t="shared" si="1"/>
+        <v>3150</v>
+      </c>
+      <c r="G132">
         <v>35</v>
       </c>
-      <c r="G132">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H132">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
@@ -3304,14 +3896,18 @@
       <c r="D133" s="2">
         <v>1500</v>
       </c>
-      <c r="F133">
+      <c r="E133" s="2">
+        <f t="shared" ref="E133:E145" si="2">ROUND(D133+5%*D133,0)</f>
+        <v>1575</v>
+      </c>
+      <c r="G133">
         <v>36</v>
       </c>
-      <c r="G133">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H133">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
@@ -3324,14 +3920,18 @@
       <c r="D134" s="2">
         <v>3000</v>
       </c>
-      <c r="F134">
+      <c r="E134" s="2">
+        <f t="shared" si="2"/>
+        <v>3150</v>
+      </c>
+      <c r="G134">
         <v>37</v>
       </c>
-      <c r="G134">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H134">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
@@ -3344,14 +3944,18 @@
       <c r="D135" s="2">
         <v>9000</v>
       </c>
-      <c r="F135">
+      <c r="E135" s="2">
+        <f t="shared" si="2"/>
+        <v>9450</v>
+      </c>
+      <c r="G135">
         <v>38</v>
       </c>
-      <c r="G135">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H135">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
@@ -3364,14 +3968,18 @@
       <c r="D136" s="2">
         <v>2500</v>
       </c>
-      <c r="F136">
+      <c r="E136" s="2">
+        <f t="shared" si="2"/>
+        <v>2625</v>
+      </c>
+      <c r="G136">
         <v>39</v>
       </c>
-      <c r="G136">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H136">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
@@ -3384,14 +3992,18 @@
       <c r="D137" s="2">
         <v>2000</v>
       </c>
-      <c r="F137">
+      <c r="E137" s="2">
+        <f t="shared" si="2"/>
+        <v>2100</v>
+      </c>
+      <c r="G137">
         <v>40</v>
       </c>
-      <c r="G137">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H137">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
@@ -3404,14 +4016,18 @@
       <c r="D138" s="2">
         <v>1500</v>
       </c>
-      <c r="F138">
+      <c r="E138" s="2">
+        <f t="shared" si="2"/>
+        <v>1575</v>
+      </c>
+      <c r="G138">
         <v>41</v>
       </c>
-      <c r="G138">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H138">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
@@ -3424,14 +4040,18 @@
       <c r="D139" s="2">
         <v>3500</v>
       </c>
-      <c r="F139">
+      <c r="E139" s="2">
+        <f t="shared" si="2"/>
+        <v>3675</v>
+      </c>
+      <c r="G139">
         <v>42</v>
       </c>
-      <c r="G139">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H139">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
@@ -3444,14 +4064,18 @@
       <c r="D140" s="2">
         <v>3000</v>
       </c>
-      <c r="F140">
+      <c r="E140" s="2">
+        <f t="shared" si="2"/>
+        <v>3150</v>
+      </c>
+      <c r="G140">
         <v>43</v>
       </c>
-      <c r="G140">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H140">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
@@ -3464,14 +4088,18 @@
       <c r="D141" s="2">
         <v>2500</v>
       </c>
-      <c r="F141">
+      <c r="E141" s="2">
+        <f t="shared" si="2"/>
+        <v>2625</v>
+      </c>
+      <c r="G141">
         <v>44</v>
       </c>
-      <c r="G141">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H141">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
@@ -3484,14 +4112,18 @@
       <c r="D142" s="2">
         <v>4000</v>
       </c>
-      <c r="F142">
+      <c r="E142" s="2">
+        <f t="shared" si="2"/>
+        <v>4200</v>
+      </c>
+      <c r="G142">
         <v>45</v>
       </c>
-      <c r="G142">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H142">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
@@ -3504,14 +4136,18 @@
       <c r="D143" s="2">
         <v>750</v>
       </c>
-      <c r="F143">
+      <c r="E143" s="2">
+        <f t="shared" si="2"/>
+        <v>788</v>
+      </c>
+      <c r="G143">
         <v>46</v>
       </c>
-      <c r="G143">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H143">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
@@ -3524,14 +4160,18 @@
       <c r="D144" s="2">
         <v>0</v>
       </c>
-      <c r="F144">
+      <c r="E144" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G144">
         <v>47</v>
       </c>
-      <c r="G144">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H144">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
@@ -3544,10 +4184,14 @@
       <c r="D145" s="2">
         <v>11000</v>
       </c>
-      <c r="F145">
+      <c r="E145" s="2">
+        <f t="shared" si="2"/>
+        <v>11550</v>
+      </c>
+      <c r="G145">
         <v>48</v>
       </c>
-      <c r="G145">
+      <c r="H145">
         <v>3</v>
       </c>
     </row>
@@ -3561,7 +4205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F49"/>
     </sheetView>
   </sheetViews>
@@ -4446,7 +5090,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -4466,10 +5110,10 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4483,10 +5127,10 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4500,10 +5144,10 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -4516,7 +5160,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4540,7 +5184,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -4560,10 +5204,10 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4577,10 +5221,10 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4594,13 +5238,244 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="1">
+        <v>41594</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="1">
+        <v>41594</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="1">
+        <v>41594</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="1">
+        <v>41594</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="1">
+        <v>41594</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="1">
+        <v>41594</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="1">
+        <v>41594</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="1">
+        <v>41594</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="1">
+        <v>41594</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>92</v>
+      </c>
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Penambahan `Bahan` (seperti linen, fiber) pada `ItemPakaian`.
</commit_message>
<xml_diff>
--- a/data_awal.xlsx
+++ b/data_awal.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="hibernate_sequences" sheetId="2" r:id="rId1"/>
     <sheet name="work" sheetId="3" r:id="rId2"/>
     <sheet name="itempakaian" sheetId="1" r:id="rId3"/>
     <sheet name="kategori" sheetId="4" r:id="rId4"/>
-    <sheet name="jeniswork" sheetId="5" r:id="rId5"/>
-    <sheet name="pelanggan" sheetId="6" r:id="rId6"/>
+    <sheet name="bahan" sheetId="7" r:id="rId5"/>
+    <sheet name="jeniswork" sheetId="5" r:id="rId6"/>
+    <sheet name="pelanggan" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="115">
   <si>
     <t>id</t>
   </si>
@@ -298,6 +299,72 @@
   </si>
   <si>
     <t>PT. SMIK</t>
+  </si>
+  <si>
+    <t>F &amp; B Linen</t>
+  </si>
+  <si>
+    <t>bahan_id</t>
+  </si>
+  <si>
+    <t>Bath Towel</t>
+  </si>
+  <si>
+    <t>Hand Towel</t>
+  </si>
+  <si>
+    <t>Face Towel</t>
+  </si>
+  <si>
+    <t>Bathrobe / Kimono</t>
+  </si>
+  <si>
+    <t>Bed Sheet King</t>
+  </si>
+  <si>
+    <t>Bed Sheet Queen</t>
+  </si>
+  <si>
+    <t>Bed Sheet Twin</t>
+  </si>
+  <si>
+    <t>Blanket / Inner Duvet</t>
+  </si>
+  <si>
+    <t>Pillowcase / Bolstercase</t>
+  </si>
+  <si>
+    <t>Skirting</t>
+  </si>
+  <si>
+    <t>Curtain</t>
+  </si>
+  <si>
+    <t>Mattress</t>
+  </si>
+  <si>
+    <t>Table Cloth</t>
+  </si>
+  <si>
+    <t>Napkin</t>
+  </si>
+  <si>
+    <t>Place Mat</t>
+  </si>
+  <si>
+    <t>Cover Chair</t>
+  </si>
+  <si>
+    <t>Overlay</t>
+  </si>
+  <si>
+    <t>Kain Satin</t>
+  </si>
+  <si>
+    <t>Valvet / Runner</t>
+  </si>
+  <si>
+    <t>Short / Celana Pendek Spa</t>
   </si>
 </sst>
 </file>
@@ -700,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection sqref="A1:H145"/>
+    <sheetView topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="E137" sqref="E137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4203,10 +4270,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F49"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4216,10 +4283,11 @@
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4236,10 +4304,13 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4252,11 +4323,11 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4269,11 +4340,11 @@
       <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4286,11 +4357,11 @@
       <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4303,11 +4374,11 @@
       <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4320,11 +4391,11 @@
       <c r="E6" t="s">
         <v>11</v>
       </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4337,11 +4408,11 @@
       <c r="E7" t="s">
         <v>12</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4354,11 +4425,11 @@
       <c r="E8" t="s">
         <v>13</v>
       </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4371,11 +4442,11 @@
       <c r="E9" t="s">
         <v>14</v>
       </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4388,11 +4459,11 @@
       <c r="E10" t="s">
         <v>15</v>
       </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4405,11 +4476,11 @@
       <c r="E11" t="s">
         <v>16</v>
       </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4422,11 +4493,11 @@
       <c r="E12" t="s">
         <v>17</v>
       </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4439,11 +4510,11 @@
       <c r="E13" t="s">
         <v>18</v>
       </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4456,11 +4527,11 @@
       <c r="E14" t="s">
         <v>19</v>
       </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4473,11 +4544,11 @@
       <c r="E15" t="s">
         <v>20</v>
       </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4490,11 +4561,11 @@
       <c r="E16" t="s">
         <v>21</v>
       </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4507,11 +4578,11 @@
       <c r="E17" t="s">
         <v>22</v>
       </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4524,11 +4595,11 @@
       <c r="E18" t="s">
         <v>23</v>
       </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4541,11 +4612,11 @@
       <c r="E19" t="s">
         <v>24</v>
       </c>
-      <c r="F19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4558,11 +4629,11 @@
       <c r="E20" t="s">
         <v>25</v>
       </c>
-      <c r="F20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4575,11 +4646,11 @@
       <c r="E21" t="s">
         <v>26</v>
       </c>
-      <c r="F21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4592,11 +4663,11 @@
       <c r="E22" t="s">
         <v>27</v>
       </c>
-      <c r="F22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4609,11 +4680,11 @@
       <c r="E23" t="s">
         <v>28</v>
       </c>
-      <c r="F23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4626,11 +4697,11 @@
       <c r="E24" t="s">
         <v>29</v>
       </c>
-      <c r="F24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4643,11 +4714,11 @@
       <c r="E25" t="s">
         <v>30</v>
       </c>
-      <c r="F25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4660,11 +4731,11 @@
       <c r="E26" t="s">
         <v>31</v>
       </c>
-      <c r="F26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4677,11 +4748,11 @@
       <c r="E27" t="s">
         <v>32</v>
       </c>
-      <c r="F27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4694,11 +4765,11 @@
       <c r="E28" t="s">
         <v>33</v>
       </c>
-      <c r="F28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4711,11 +4782,11 @@
       <c r="E29" t="s">
         <v>34</v>
       </c>
-      <c r="F29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4728,11 +4799,11 @@
       <c r="E30" t="s">
         <v>35</v>
       </c>
-      <c r="F30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4745,11 +4816,11 @@
       <c r="E31" t="s">
         <v>36</v>
       </c>
-      <c r="F31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4762,11 +4833,11 @@
       <c r="E32" t="s">
         <v>37</v>
       </c>
-      <c r="F32">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4779,11 +4850,11 @@
       <c r="E33" t="s">
         <v>38</v>
       </c>
-      <c r="F33">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4796,11 +4867,11 @@
       <c r="E34" t="s">
         <v>39</v>
       </c>
-      <c r="F34">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4813,11 +4884,11 @@
       <c r="E35" t="s">
         <v>40</v>
       </c>
-      <c r="F35">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4830,11 +4901,11 @@
       <c r="E36" t="s">
         <v>41</v>
       </c>
-      <c r="F36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4847,11 +4918,11 @@
       <c r="E37" t="s">
         <v>42</v>
       </c>
-      <c r="F37">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4864,11 +4935,11 @@
       <c r="E38" t="s">
         <v>43</v>
       </c>
-      <c r="F38">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4881,11 +4952,11 @@
       <c r="E39" t="s">
         <v>44</v>
       </c>
-      <c r="F39">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4898,11 +4969,11 @@
       <c r="E40" t="s">
         <v>45</v>
       </c>
-      <c r="F40">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4915,11 +4986,11 @@
       <c r="E41" t="s">
         <v>46</v>
       </c>
-      <c r="F41">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4932,11 +5003,11 @@
       <c r="E42" t="s">
         <v>47</v>
       </c>
-      <c r="F42">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4949,11 +5020,11 @@
       <c r="E43" t="s">
         <v>48</v>
       </c>
-      <c r="F43">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4966,11 +5037,11 @@
       <c r="E44" t="s">
         <v>49</v>
       </c>
-      <c r="F44">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4983,11 +5054,11 @@
       <c r="E45" t="s">
         <v>50</v>
       </c>
-      <c r="F45">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5000,11 +5071,11 @@
       <c r="E46" t="s">
         <v>51</v>
       </c>
-      <c r="F46">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5017,11 +5088,11 @@
       <c r="E47" t="s">
         <v>52</v>
       </c>
-      <c r="F47">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5034,11 +5105,11 @@
       <c r="E48" t="s">
         <v>53</v>
       </c>
-      <c r="F48">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -5051,8 +5122,433 @@
       <c r="E49" t="s">
         <v>54</v>
       </c>
-      <c r="F49">
-        <v>3</v>
+      <c r="G49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" t="s">
+        <v>95</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C51" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" t="s">
+        <v>96</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C52" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" t="s">
+        <v>97</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C53" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" t="s">
+        <v>43</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C54" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" t="s">
+        <v>40</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C55" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" t="s">
+        <v>98</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C56" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" t="s">
+        <v>99</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C57" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" t="s">
+        <v>100</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C58" t="s">
+        <v>6</v>
+      </c>
+      <c r="E58" t="s">
+        <v>101</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C59" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" t="s">
+        <v>48</v>
+      </c>
+      <c r="F59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C60" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" t="s">
+        <v>49</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C61" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61" t="s">
+        <v>50</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C62" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62" t="s">
+        <v>102</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C63" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63" t="s">
+        <v>103</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C64" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" t="s">
+        <v>104</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C65" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" t="s">
+        <v>105</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C66" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66" t="s">
+        <v>106</v>
+      </c>
+      <c r="F66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C67" t="s">
+        <v>6</v>
+      </c>
+      <c r="E67" t="s">
+        <v>107</v>
+      </c>
+      <c r="F67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C68" t="s">
+        <v>6</v>
+      </c>
+      <c r="E68" t="s">
+        <v>108</v>
+      </c>
+      <c r="F68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C69" t="s">
+        <v>6</v>
+      </c>
+      <c r="E69" t="s">
+        <v>109</v>
+      </c>
+      <c r="F69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C70" t="s">
+        <v>6</v>
+      </c>
+      <c r="E70" t="s">
+        <v>110</v>
+      </c>
+      <c r="F70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C71" t="s">
+        <v>6</v>
+      </c>
+      <c r="E71" t="s">
+        <v>111</v>
+      </c>
+      <c r="F71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C72" t="s">
+        <v>6</v>
+      </c>
+      <c r="E72" t="s">
+        <v>112</v>
+      </c>
+      <c r="F72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C73" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73" t="s">
+        <v>113</v>
+      </c>
+      <c r="F73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C74" t="s">
+        <v>6</v>
+      </c>
+      <c r="E74" t="s">
+        <v>114</v>
+      </c>
+      <c r="F74">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -5157,6 +5653,84 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>41643.677407407406</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>41643.677465277775</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5249,7 +5823,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>

</xml_diff>

<commit_message>
Mengubah tampilan pencarian dan informasi pada daftar harga.
</commit_message>
<xml_diff>
--- a/data_awal.xlsx
+++ b/data_awal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="hibernate_sequences" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="115">
   <si>
     <t>id</t>
   </si>
@@ -765,10 +765,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H145"/>
+  <dimension ref="A1:H220"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="E137" sqref="E137"/>
+    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,7 +892,7 @@
         <v>11000</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" ref="E5:E68" si="0">ROUND(D5+5%*D5,0)</f>
+        <f t="shared" ref="E5:E93" si="0">ROUND(D5+5%*D5,0)</f>
         <v>11550</v>
       </c>
       <c r="G5">
@@ -1969,17 +1969,17 @@
         <v>6</v>
       </c>
       <c r="D50" s="2">
-        <v>22500</v>
+        <v>4300</v>
       </c>
       <c r="E50" s="2">
         <f t="shared" si="0"/>
-        <v>23625</v>
+        <v>4515</v>
       </c>
       <c r="G50">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="H50">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -1993,17 +1993,17 @@
         <v>6</v>
       </c>
       <c r="D51" s="2">
-        <v>16000</v>
+        <v>2500</v>
       </c>
       <c r="E51" s="2">
         <f t="shared" si="0"/>
-        <v>16800</v>
+        <v>2625</v>
       </c>
       <c r="G51">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="H51">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -2017,17 +2017,17 @@
         <v>6</v>
       </c>
       <c r="D52" s="2">
-        <v>21500</v>
+        <v>2000</v>
       </c>
       <c r="E52" s="2">
         <f t="shared" si="0"/>
-        <v>22575</v>
+        <v>2100</v>
       </c>
       <c r="G52">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="H52">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -2041,17 +2041,17 @@
         <v>6</v>
       </c>
       <c r="D53" s="2">
-        <v>12000</v>
+        <v>7000</v>
       </c>
       <c r="E53" s="2">
         <f t="shared" si="0"/>
-        <v>12600</v>
+        <v>7350</v>
       </c>
       <c r="G53">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="H53">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -2065,17 +2065,17 @@
         <v>6</v>
       </c>
       <c r="D54" s="2">
-        <v>15000</v>
+        <v>3500</v>
       </c>
       <c r="E54" s="2">
         <f t="shared" si="0"/>
-        <v>15750</v>
+        <v>3675</v>
       </c>
       <c r="G54">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="H54">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -2089,17 +2089,17 @@
         <v>6</v>
       </c>
       <c r="D55" s="2">
-        <v>13000</v>
+        <v>10500</v>
       </c>
       <c r="E55" s="2">
         <f t="shared" si="0"/>
-        <v>13650</v>
+        <v>11025</v>
       </c>
       <c r="G55">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="H55">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -2113,17 +2113,17 @@
         <v>6</v>
       </c>
       <c r="D56" s="2">
-        <v>15500</v>
+        <v>3500</v>
       </c>
       <c r="E56" s="2">
         <f t="shared" si="0"/>
-        <v>16275</v>
+        <v>3675</v>
       </c>
       <c r="G56">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="H56">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -2137,17 +2137,17 @@
         <v>6</v>
       </c>
       <c r="D57" s="2">
-        <v>15000</v>
+        <v>3000</v>
       </c>
       <c r="E57" s="2">
         <f t="shared" si="0"/>
-        <v>15750</v>
+        <v>3150</v>
       </c>
       <c r="G57">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="H57">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -2161,17 +2161,17 @@
         <v>6</v>
       </c>
       <c r="D58" s="2">
-        <v>13000</v>
+        <v>2500</v>
       </c>
       <c r="E58" s="2">
         <f t="shared" si="0"/>
-        <v>13650</v>
+        <v>2625</v>
       </c>
       <c r="G58">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="H58">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -2185,17 +2185,17 @@
         <v>6</v>
       </c>
       <c r="D59" s="2">
-        <v>15500</v>
+        <v>4500</v>
       </c>
       <c r="E59" s="2">
         <f t="shared" si="0"/>
-        <v>16275</v>
+        <v>4725</v>
       </c>
       <c r="G59">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="H59">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -2209,17 +2209,17 @@
         <v>6</v>
       </c>
       <c r="D60" s="2">
-        <v>15000</v>
+        <v>4000</v>
       </c>
       <c r="E60" s="2">
         <f t="shared" si="0"/>
-        <v>15750</v>
+        <v>4200</v>
       </c>
       <c r="G60">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="H60">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -2233,17 +2233,17 @@
         <v>6</v>
       </c>
       <c r="D61" s="2">
-        <v>13000</v>
+        <v>3500</v>
       </c>
       <c r="E61" s="2">
         <f t="shared" si="0"/>
-        <v>13650</v>
+        <v>3675</v>
       </c>
       <c r="G61">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="H61">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -2257,17 +2257,17 @@
         <v>6</v>
       </c>
       <c r="D62" s="2">
-        <v>9000</v>
+        <v>6000</v>
       </c>
       <c r="E62" s="2">
         <f t="shared" si="0"/>
-        <v>9450</v>
+        <v>6300</v>
       </c>
       <c r="G62">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="H62">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -2281,17 +2281,17 @@
         <v>6</v>
       </c>
       <c r="D63" s="2">
-        <v>9000</v>
+        <v>2000</v>
       </c>
       <c r="E63" s="2">
         <f t="shared" si="0"/>
-        <v>9450</v>
+        <v>2100</v>
       </c>
       <c r="G63">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="H63">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -2305,17 +2305,17 @@
         <v>6</v>
       </c>
       <c r="D64" s="2">
-        <v>8000</v>
+        <v>4000</v>
       </c>
       <c r="E64" s="2">
         <f t="shared" si="0"/>
-        <v>8400</v>
+        <v>4200</v>
       </c>
       <c r="G64">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="H64">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -2329,17 +2329,17 @@
         <v>6</v>
       </c>
       <c r="D65" s="2">
-        <v>0</v>
+        <v>12500</v>
       </c>
       <c r="E65" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13125</v>
       </c>
       <c r="G65">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="H65">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -2353,17 +2353,17 @@
         <v>6</v>
       </c>
       <c r="D66" s="2">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="E66" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15750</v>
       </c>
       <c r="G66">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="H66">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -2377,17 +2377,17 @@
         <v>6</v>
       </c>
       <c r="D67" s="2">
-        <v>16500</v>
+        <v>4000</v>
       </c>
       <c r="E67" s="2">
         <f t="shared" si="0"/>
-        <v>17325</v>
+        <v>4200</v>
       </c>
       <c r="G67">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="H67">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -2401,17 +2401,17 @@
         <v>6</v>
       </c>
       <c r="D68" s="2">
-        <v>14500</v>
+        <v>2200</v>
       </c>
       <c r="E68" s="2">
         <f t="shared" si="0"/>
-        <v>15225</v>
+        <v>2310</v>
       </c>
       <c r="G68">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="H68">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -2425,17 +2425,17 @@
         <v>6</v>
       </c>
       <c r="D69" s="2">
-        <v>7500</v>
+        <v>2200</v>
       </c>
       <c r="E69" s="2">
-        <f t="shared" ref="E69:E132" si="1">ROUND(D69+5%*D69,0)</f>
-        <v>7875</v>
+        <f t="shared" si="0"/>
+        <v>2310</v>
       </c>
       <c r="G69">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="H69">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -2449,17 +2449,17 @@
         <v>6</v>
       </c>
       <c r="D70" s="2">
-        <v>23500</v>
+        <v>3500</v>
       </c>
       <c r="E70" s="2">
-        <f t="shared" si="1"/>
-        <v>24675</v>
+        <f t="shared" si="0"/>
+        <v>3675</v>
       </c>
       <c r="G70">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="H70">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -2473,17 +2473,17 @@
         <v>6</v>
       </c>
       <c r="D71" s="2">
-        <v>19000</v>
+        <v>4000</v>
       </c>
       <c r="E71" s="2">
-        <f t="shared" si="1"/>
-        <v>19950</v>
+        <f t="shared" si="0"/>
+        <v>4200</v>
       </c>
       <c r="G71">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="H71">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -2497,17 +2497,17 @@
         <v>6</v>
       </c>
       <c r="D72" s="2">
-        <v>17500</v>
+        <v>7000</v>
       </c>
       <c r="E72" s="2">
-        <f t="shared" si="1"/>
-        <v>18375</v>
+        <f t="shared" si="0"/>
+        <v>7350</v>
       </c>
       <c r="G72">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="H72">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -2521,17 +2521,17 @@
         <v>6</v>
       </c>
       <c r="D73" s="2">
-        <v>22500</v>
+        <v>4000</v>
       </c>
       <c r="E73" s="2">
-        <f t="shared" si="1"/>
-        <v>23625</v>
+        <f t="shared" si="0"/>
+        <v>4200</v>
       </c>
       <c r="G73">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="H73">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -2545,17 +2545,17 @@
         <v>6</v>
       </c>
       <c r="D74" s="2">
-        <v>30000</v>
+        <v>11000</v>
       </c>
       <c r="E74" s="2">
-        <f t="shared" si="1"/>
-        <v>31500</v>
+        <f t="shared" si="0"/>
+        <v>11550</v>
       </c>
       <c r="G74">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="H74">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -2569,14 +2569,14 @@
         <v>6</v>
       </c>
       <c r="D75" s="2">
-        <v>26000</v>
+        <v>22500</v>
       </c>
       <c r="E75" s="2">
-        <f t="shared" si="1"/>
-        <v>27300</v>
+        <f t="shared" si="0"/>
+        <v>23625</v>
       </c>
       <c r="G75">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="H75">
         <v>2</v>
@@ -2593,14 +2593,14 @@
         <v>6</v>
       </c>
       <c r="D76" s="2">
-        <v>35500</v>
+        <v>16000</v>
       </c>
       <c r="E76" s="2">
-        <f t="shared" si="1"/>
-        <v>37275</v>
+        <f t="shared" si="0"/>
+        <v>16800</v>
       </c>
       <c r="G76">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="H76">
         <v>2</v>
@@ -2617,14 +2617,14 @@
         <v>6</v>
       </c>
       <c r="D77" s="2">
-        <v>44500</v>
+        <v>21500</v>
       </c>
       <c r="E77" s="2">
-        <f t="shared" si="1"/>
-        <v>46725</v>
+        <f t="shared" si="0"/>
+        <v>22575</v>
       </c>
       <c r="G77">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="H77">
         <v>2</v>
@@ -2641,14 +2641,14 @@
         <v>6</v>
       </c>
       <c r="D78" s="2">
-        <v>20500</v>
+        <v>12000</v>
       </c>
       <c r="E78" s="2">
-        <f t="shared" si="1"/>
-        <v>21525</v>
+        <f t="shared" si="0"/>
+        <v>12600</v>
       </c>
       <c r="G78">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="H78">
         <v>2</v>
@@ -2665,14 +2665,14 @@
         <v>6</v>
       </c>
       <c r="D79" s="2">
-        <v>34500</v>
+        <v>15000</v>
       </c>
       <c r="E79" s="2">
-        <f t="shared" si="1"/>
-        <v>36225</v>
+        <f t="shared" si="0"/>
+        <v>15750</v>
       </c>
       <c r="G79">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="H79">
         <v>2</v>
@@ -2689,14 +2689,14 @@
         <v>6</v>
       </c>
       <c r="D80" s="2">
-        <v>9500</v>
+        <v>13000</v>
       </c>
       <c r="E80" s="2">
-        <f t="shared" si="1"/>
-        <v>9975</v>
+        <f t="shared" si="0"/>
+        <v>13650</v>
       </c>
       <c r="G80">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="H80">
         <v>2</v>
@@ -2716,11 +2716,11 @@
         <v>15500</v>
       </c>
       <c r="E81" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16275</v>
       </c>
       <c r="G81">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="H81">
         <v>2</v>
@@ -2737,14 +2737,14 @@
         <v>6</v>
       </c>
       <c r="D82" s="2">
-        <v>8500</v>
+        <v>15000</v>
       </c>
       <c r="E82" s="2">
-        <f t="shared" si="1"/>
-        <v>8925</v>
+        <f t="shared" si="0"/>
+        <v>15750</v>
       </c>
       <c r="G82">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="H82">
         <v>2</v>
@@ -2761,14 +2761,14 @@
         <v>6</v>
       </c>
       <c r="D83" s="2">
-        <v>0</v>
+        <v>13000</v>
       </c>
       <c r="E83" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>13650</v>
       </c>
       <c r="G83">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="H83">
         <v>2</v>
@@ -2785,14 +2785,14 @@
         <v>6</v>
       </c>
       <c r="D84" s="2">
-        <v>0</v>
+        <v>15500</v>
       </c>
       <c r="E84" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>16275</v>
       </c>
       <c r="G84">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="H84">
         <v>2</v>
@@ -2809,14 +2809,14 @@
         <v>6</v>
       </c>
       <c r="D85" s="2">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="E85" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>15750</v>
       </c>
       <c r="G85">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="H85">
         <v>2</v>
@@ -2833,14 +2833,14 @@
         <v>6</v>
       </c>
       <c r="D86" s="2">
-        <v>0</v>
+        <v>13000</v>
       </c>
       <c r="E86" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>13650</v>
       </c>
       <c r="G86">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="H86">
         <v>2</v>
@@ -2857,14 +2857,14 @@
         <v>6</v>
       </c>
       <c r="D87" s="2">
-        <v>0</v>
+        <v>9000</v>
       </c>
       <c r="E87" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>9450</v>
       </c>
       <c r="G87">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="H87">
         <v>2</v>
@@ -2881,14 +2881,14 @@
         <v>6</v>
       </c>
       <c r="D88" s="2">
-        <v>0</v>
+        <v>9000</v>
       </c>
       <c r="E88" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>9450</v>
       </c>
       <c r="G88">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="H88">
         <v>2</v>
@@ -2905,14 +2905,14 @@
         <v>6</v>
       </c>
       <c r="D89" s="2">
-        <v>0</v>
+        <v>8000</v>
       </c>
       <c r="E89" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>8400</v>
       </c>
       <c r="G89">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="H89">
         <v>2</v>
@@ -2932,11 +2932,11 @@
         <v>0</v>
       </c>
       <c r="E90" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G90">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="H90">
         <v>2</v>
@@ -2956,11 +2956,11 @@
         <v>0</v>
       </c>
       <c r="E91" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G91">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="H91">
         <v>2</v>
@@ -2977,14 +2977,14 @@
         <v>6</v>
       </c>
       <c r="D92" s="2">
-        <v>0</v>
+        <v>16500</v>
       </c>
       <c r="E92" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>17325</v>
       </c>
       <c r="G92">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="H92">
         <v>2</v>
@@ -3001,14 +3001,14 @@
         <v>6</v>
       </c>
       <c r="D93" s="2">
-        <v>0</v>
+        <v>14500</v>
       </c>
       <c r="E93" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>15225</v>
       </c>
       <c r="G93">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="H93">
         <v>2</v>
@@ -3025,14 +3025,14 @@
         <v>6</v>
       </c>
       <c r="D94" s="2">
-        <v>8000</v>
+        <v>7500</v>
       </c>
       <c r="E94" s="2">
-        <f t="shared" si="1"/>
-        <v>8400</v>
+        <f t="shared" ref="E94:E182" si="1">ROUND(D94+5%*D94,0)</f>
+        <v>7875</v>
       </c>
       <c r="G94">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="H94">
         <v>2</v>
@@ -3049,14 +3049,14 @@
         <v>6</v>
       </c>
       <c r="D95" s="2">
-        <v>0</v>
+        <v>23500</v>
       </c>
       <c r="E95" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>24675</v>
       </c>
       <c r="G95">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="H95">
         <v>2</v>
@@ -3073,14 +3073,14 @@
         <v>6</v>
       </c>
       <c r="D96" s="2">
-        <v>0</v>
+        <v>19000</v>
       </c>
       <c r="E96" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>19950</v>
       </c>
       <c r="G96">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="H96">
         <v>2</v>
@@ -3097,14 +3097,14 @@
         <v>6</v>
       </c>
       <c r="D97" s="2">
-        <v>15000</v>
+        <v>17500</v>
       </c>
       <c r="E97" s="2">
         <f t="shared" si="1"/>
-        <v>15750</v>
+        <v>18375</v>
       </c>
       <c r="G97">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="H97">
         <v>2</v>
@@ -3121,17 +3121,17 @@
         <v>6</v>
       </c>
       <c r="D98" s="2">
-        <v>16000</v>
+        <v>22500</v>
       </c>
       <c r="E98" s="2">
         <f t="shared" si="1"/>
-        <v>16800</v>
+        <v>23625</v>
       </c>
       <c r="G98">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="H98">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -3145,17 +3145,17 @@
         <v>6</v>
       </c>
       <c r="D99" s="2">
-        <v>11000</v>
+        <v>30000</v>
       </c>
       <c r="E99" s="2">
         <f t="shared" si="1"/>
-        <v>11550</v>
+        <v>31500</v>
       </c>
       <c r="G99">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="H99">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -3169,17 +3169,17 @@
         <v>6</v>
       </c>
       <c r="D100" s="2">
-        <v>15500</v>
+        <v>26000</v>
       </c>
       <c r="E100" s="2">
         <f t="shared" si="1"/>
-        <v>16275</v>
+        <v>27300</v>
       </c>
       <c r="G100">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="H100">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -3193,17 +3193,17 @@
         <v>6</v>
       </c>
       <c r="D101" s="2">
-        <v>7500</v>
+        <v>35500</v>
       </c>
       <c r="E101" s="2">
         <f t="shared" si="1"/>
-        <v>7875</v>
+        <v>37275</v>
       </c>
       <c r="G101">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="H101">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -3217,17 +3217,17 @@
         <v>6</v>
       </c>
       <c r="D102" s="2">
-        <v>8500</v>
+        <v>44500</v>
       </c>
       <c r="E102" s="2">
         <f t="shared" si="1"/>
-        <v>8925</v>
+        <v>46725</v>
       </c>
       <c r="G102">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="H102">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -3241,17 +3241,17 @@
         <v>6</v>
       </c>
       <c r="D103" s="2">
-        <v>7000</v>
+        <v>20500</v>
       </c>
       <c r="E103" s="2">
         <f t="shared" si="1"/>
-        <v>7350</v>
+        <v>21525</v>
       </c>
       <c r="G103">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="H103">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -3265,17 +3265,17 @@
         <v>6</v>
       </c>
       <c r="D104" s="2">
-        <v>9500</v>
+        <v>34500</v>
       </c>
       <c r="E104" s="2">
         <f t="shared" si="1"/>
-        <v>9975</v>
+        <v>36225</v>
       </c>
       <c r="G104">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="H104">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -3289,17 +3289,17 @@
         <v>6</v>
       </c>
       <c r="D105" s="2">
-        <v>8500</v>
+        <v>9500</v>
       </c>
       <c r="E105" s="2">
         <f t="shared" si="1"/>
-        <v>8925</v>
+        <v>9975</v>
       </c>
       <c r="G105">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="H105">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -3313,17 +3313,17 @@
         <v>6</v>
       </c>
       <c r="D106" s="2">
-        <v>7000</v>
+        <v>15500</v>
       </c>
       <c r="E106" s="2">
         <f t="shared" si="1"/>
-        <v>7350</v>
+        <v>16275</v>
       </c>
       <c r="G106">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="H106">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -3337,17 +3337,17 @@
         <v>6</v>
       </c>
       <c r="D107" s="2">
-        <v>5000</v>
+        <v>8500</v>
       </c>
       <c r="E107" s="2">
         <f t="shared" si="1"/>
-        <v>5250</v>
+        <v>8925</v>
       </c>
       <c r="G107">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="H107">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -3361,17 +3361,17 @@
         <v>6</v>
       </c>
       <c r="D108" s="2">
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="E108" s="2">
         <f t="shared" si="1"/>
-        <v>6300</v>
+        <v>0</v>
       </c>
       <c r="G108">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="H108">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -3385,17 +3385,17 @@
         <v>6</v>
       </c>
       <c r="D109" s="2">
-        <v>3050</v>
+        <v>0</v>
       </c>
       <c r="E109" s="2">
         <f t="shared" si="1"/>
-        <v>3203</v>
+        <v>0</v>
       </c>
       <c r="G109">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="H109">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -3409,17 +3409,17 @@
         <v>6</v>
       </c>
       <c r="D110" s="2">
-        <v>11000</v>
+        <v>0</v>
       </c>
       <c r="E110" s="2">
         <f t="shared" si="1"/>
-        <v>11550</v>
+        <v>0</v>
       </c>
       <c r="G110">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="H110">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -3433,17 +3433,17 @@
         <v>6</v>
       </c>
       <c r="D111" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="E111" s="2">
         <f t="shared" si="1"/>
-        <v>2100</v>
+        <v>0</v>
       </c>
       <c r="G111">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="H111">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -3457,17 +3457,17 @@
         <v>6</v>
       </c>
       <c r="D112" s="2">
-        <v>10500</v>
+        <v>0</v>
       </c>
       <c r="E112" s="2">
         <f t="shared" si="1"/>
-        <v>11025</v>
+        <v>0</v>
       </c>
       <c r="G112">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="H112">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -3481,17 +3481,17 @@
         <v>6</v>
       </c>
       <c r="D113" s="2">
-        <v>6500</v>
+        <v>0</v>
       </c>
       <c r="E113" s="2">
         <f t="shared" si="1"/>
-        <v>6825</v>
+        <v>0</v>
       </c>
       <c r="G113">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="H113">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -3505,17 +3505,17 @@
         <v>6</v>
       </c>
       <c r="D114" s="2">
-        <v>4500</v>
+        <v>0</v>
       </c>
       <c r="E114" s="2">
         <f t="shared" si="1"/>
-        <v>4725</v>
+        <v>0</v>
       </c>
       <c r="G114">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="H114">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -3529,17 +3529,17 @@
         <v>6</v>
       </c>
       <c r="D115" s="2">
-        <v>15500</v>
+        <v>0</v>
       </c>
       <c r="E115" s="2">
         <f t="shared" si="1"/>
-        <v>16275</v>
+        <v>0</v>
       </c>
       <c r="G115">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="H115">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -3553,17 +3553,17 @@
         <v>6</v>
       </c>
       <c r="D116" s="2">
-        <v>9500</v>
+        <v>0</v>
       </c>
       <c r="E116" s="2">
         <f t="shared" si="1"/>
-        <v>9975</v>
+        <v>0</v>
       </c>
       <c r="G116">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="H116">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -3577,17 +3577,17 @@
         <v>6</v>
       </c>
       <c r="D117" s="2">
-        <v>9500</v>
+        <v>0</v>
       </c>
       <c r="E117" s="2">
         <f t="shared" si="1"/>
-        <v>9975</v>
+        <v>0</v>
       </c>
       <c r="G117">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="H117">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -3601,17 +3601,17 @@
         <v>6</v>
       </c>
       <c r="D118" s="2">
-        <v>12500</v>
+        <v>0</v>
       </c>
       <c r="E118" s="2">
         <f t="shared" si="1"/>
-        <v>13125</v>
+        <v>0</v>
       </c>
       <c r="G118">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="H118">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -3625,17 +3625,17 @@
         <v>6</v>
       </c>
       <c r="D119" s="2">
-        <v>21000</v>
+        <v>8000</v>
       </c>
       <c r="E119" s="2">
         <f t="shared" si="1"/>
-        <v>22050</v>
+        <v>8400</v>
       </c>
       <c r="G119">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="H119">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -3649,17 +3649,17 @@
         <v>6</v>
       </c>
       <c r="D120" s="2">
-        <v>19000</v>
+        <v>0</v>
       </c>
       <c r="E120" s="2">
         <f t="shared" si="1"/>
-        <v>19950</v>
+        <v>0</v>
       </c>
       <c r="G120">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="H120">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -3673,17 +3673,17 @@
         <v>6</v>
       </c>
       <c r="D121" s="2">
-        <v>29500</v>
+        <v>0</v>
       </c>
       <c r="E121" s="2">
         <f t="shared" si="1"/>
-        <v>30975</v>
+        <v>0</v>
       </c>
       <c r="G121">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="H121">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -3697,17 +3697,17 @@
         <v>6</v>
       </c>
       <c r="D122" s="2">
-        <v>39500</v>
+        <v>15000</v>
       </c>
       <c r="E122" s="2">
         <f t="shared" si="1"/>
-        <v>41475</v>
+        <v>15750</v>
       </c>
       <c r="G122">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="H122">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -3721,17 +3721,17 @@
         <v>6</v>
       </c>
       <c r="D123" s="2">
-        <v>12500</v>
+        <v>0</v>
       </c>
       <c r="E123" s="2">
         <f t="shared" si="1"/>
-        <v>13125</v>
+        <v>0</v>
       </c>
       <c r="G123">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="H123">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -3745,17 +3745,17 @@
         <v>6</v>
       </c>
       <c r="D124" s="2">
-        <v>20500</v>
+        <v>0</v>
       </c>
       <c r="E124" s="2">
         <f t="shared" si="1"/>
-        <v>21525</v>
+        <v>0</v>
       </c>
       <c r="G124">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="H124">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -3769,17 +3769,17 @@
         <v>6</v>
       </c>
       <c r="D125" s="2">
-        <v>5500</v>
+        <v>0</v>
       </c>
       <c r="E125" s="2">
         <f t="shared" si="1"/>
-        <v>5775</v>
+        <v>0</v>
       </c>
       <c r="G125">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="H125">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -3793,17 +3793,17 @@
         <v>6</v>
       </c>
       <c r="D126" s="2">
-        <v>6500</v>
+        <v>0</v>
       </c>
       <c r="E126" s="2">
         <f t="shared" si="1"/>
-        <v>6825</v>
+        <v>0</v>
       </c>
       <c r="G126">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="H126">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -3817,17 +3817,17 @@
         <v>6</v>
       </c>
       <c r="D127" s="2">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="E127" s="2">
         <f t="shared" si="1"/>
-        <v>4200</v>
+        <v>0</v>
       </c>
       <c r="G127">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="H127">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -3841,17 +3841,17 @@
         <v>6</v>
       </c>
       <c r="D128" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="E128" s="2">
         <f t="shared" si="1"/>
-        <v>3150</v>
+        <v>0</v>
       </c>
       <c r="G128">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="H128">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -3865,17 +3865,17 @@
         <v>6</v>
       </c>
       <c r="D129" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="E129" s="2">
         <f t="shared" si="1"/>
-        <v>2100</v>
+        <v>0</v>
       </c>
       <c r="G129">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="H129">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -3889,17 +3889,17 @@
         <v>6</v>
       </c>
       <c r="D130" s="2">
-        <v>1500</v>
+        <v>0</v>
       </c>
       <c r="E130" s="2">
         <f t="shared" si="1"/>
-        <v>1575</v>
+        <v>0</v>
       </c>
       <c r="G130">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="H130">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -3913,17 +3913,17 @@
         <v>6</v>
       </c>
       <c r="D131" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="E131" s="2">
         <f t="shared" si="1"/>
-        <v>2100</v>
+        <v>0</v>
       </c>
       <c r="G131">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="H131">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -3937,17 +3937,17 @@
         <v>6</v>
       </c>
       <c r="D132" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="E132" s="2">
         <f t="shared" si="1"/>
-        <v>3150</v>
+        <v>0</v>
       </c>
       <c r="G132">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="H132">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -3961,17 +3961,17 @@
         <v>6</v>
       </c>
       <c r="D133" s="2">
-        <v>1500</v>
+        <v>0</v>
       </c>
       <c r="E133" s="2">
-        <f t="shared" ref="E133:E145" si="2">ROUND(D133+5%*D133,0)</f>
-        <v>1575</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="G133">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H133">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
@@ -3985,17 +3985,17 @@
         <v>6</v>
       </c>
       <c r="D134" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="E134" s="2">
-        <f t="shared" si="2"/>
-        <v>3150</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="G134">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="H134">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
@@ -4009,17 +4009,17 @@
         <v>6</v>
       </c>
       <c r="D135" s="2">
-        <v>9000</v>
+        <v>0</v>
       </c>
       <c r="E135" s="2">
-        <f t="shared" si="2"/>
-        <v>9450</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="G135">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="H135">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -4033,17 +4033,17 @@
         <v>6</v>
       </c>
       <c r="D136" s="2">
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="E136" s="2">
-        <f t="shared" si="2"/>
-        <v>2625</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="G136">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="H136">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -4057,17 +4057,17 @@
         <v>6</v>
       </c>
       <c r="D137" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="E137" s="2">
-        <f t="shared" si="2"/>
-        <v>2100</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="G137">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="H137">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
@@ -4081,17 +4081,17 @@
         <v>6</v>
       </c>
       <c r="D138" s="2">
-        <v>1500</v>
+        <v>0</v>
       </c>
       <c r="E138" s="2">
-        <f t="shared" si="2"/>
-        <v>1575</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="G138">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="H138">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -4105,17 +4105,17 @@
         <v>6</v>
       </c>
       <c r="D139" s="2">
-        <v>3500</v>
+        <v>0</v>
       </c>
       <c r="E139" s="2">
-        <f t="shared" si="2"/>
-        <v>3675</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="G139">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="H139">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
@@ -4129,17 +4129,17 @@
         <v>6</v>
       </c>
       <c r="D140" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="E140" s="2">
-        <f t="shared" si="2"/>
-        <v>3150</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="G140">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="H140">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
@@ -4153,17 +4153,17 @@
         <v>6</v>
       </c>
       <c r="D141" s="2">
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="E141" s="2">
-        <f t="shared" si="2"/>
-        <v>2625</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="G141">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="H141">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
@@ -4177,17 +4177,17 @@
         <v>6</v>
       </c>
       <c r="D142" s="2">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="E142" s="2">
-        <f t="shared" si="2"/>
-        <v>4200</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="G142">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="H142">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
@@ -4201,17 +4201,17 @@
         <v>6</v>
       </c>
       <c r="D143" s="2">
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="E143" s="2">
-        <f t="shared" si="2"/>
-        <v>788</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="G143">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="H143">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
@@ -4228,14 +4228,14 @@
         <v>0</v>
       </c>
       <c r="E144" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G144">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="H144">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
@@ -4249,16 +4249,1816 @@
         <v>6</v>
       </c>
       <c r="D145" s="2">
+        <v>0</v>
+      </c>
+      <c r="E145" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G145">
+        <v>71</v>
+      </c>
+      <c r="H145">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>145</v>
+      </c>
+      <c r="B146" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C146" t="s">
+        <v>6</v>
+      </c>
+      <c r="D146" s="2">
+        <v>0</v>
+      </c>
+      <c r="E146" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G146">
+        <v>72</v>
+      </c>
+      <c r="H146">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>146</v>
+      </c>
+      <c r="B147" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C147" t="s">
+        <v>6</v>
+      </c>
+      <c r="D147" s="2">
+        <v>0</v>
+      </c>
+      <c r="E147" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G147">
+        <v>73</v>
+      </c>
+      <c r="H147">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>147</v>
+      </c>
+      <c r="B148" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C148" t="s">
+        <v>6</v>
+      </c>
+      <c r="D148" s="2">
+        <v>16000</v>
+      </c>
+      <c r="E148" s="2">
+        <f t="shared" si="1"/>
+        <v>16800</v>
+      </c>
+      <c r="G148">
+        <v>1</v>
+      </c>
+      <c r="H148">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="B149" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C149" t="s">
+        <v>6</v>
+      </c>
+      <c r="D149" s="2">
         <v>11000</v>
       </c>
-      <c r="E145" s="2">
+      <c r="E149" s="2">
+        <f t="shared" si="1"/>
+        <v>11550</v>
+      </c>
+      <c r="G149">
+        <v>2</v>
+      </c>
+      <c r="H149">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="B150" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C150" t="s">
+        <v>6</v>
+      </c>
+      <c r="D150" s="2">
+        <v>15500</v>
+      </c>
+      <c r="E150" s="2">
+        <f t="shared" si="1"/>
+        <v>16275</v>
+      </c>
+      <c r="G150">
+        <v>3</v>
+      </c>
+      <c r="H150">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="B151" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C151" t="s">
+        <v>6</v>
+      </c>
+      <c r="D151" s="2">
+        <v>7500</v>
+      </c>
+      <c r="E151" s="2">
+        <f t="shared" si="1"/>
+        <v>7875</v>
+      </c>
+      <c r="G151">
+        <v>4</v>
+      </c>
+      <c r="H151">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>151</v>
+      </c>
+      <c r="B152" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C152" t="s">
+        <v>6</v>
+      </c>
+      <c r="D152" s="2">
+        <v>8500</v>
+      </c>
+      <c r="E152" s="2">
+        <f t="shared" si="1"/>
+        <v>8925</v>
+      </c>
+      <c r="G152">
+        <v>5</v>
+      </c>
+      <c r="H152">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>152</v>
+      </c>
+      <c r="B153" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C153" t="s">
+        <v>6</v>
+      </c>
+      <c r="D153" s="2">
+        <v>7000</v>
+      </c>
+      <c r="E153" s="2">
+        <f t="shared" si="1"/>
+        <v>7350</v>
+      </c>
+      <c r="G153">
+        <v>6</v>
+      </c>
+      <c r="H153">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>153</v>
+      </c>
+      <c r="B154" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C154" t="s">
+        <v>6</v>
+      </c>
+      <c r="D154" s="2">
+        <v>9500</v>
+      </c>
+      <c r="E154" s="2">
+        <f t="shared" si="1"/>
+        <v>9975</v>
+      </c>
+      <c r="G154">
+        <v>7</v>
+      </c>
+      <c r="H154">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>154</v>
+      </c>
+      <c r="B155" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C155" t="s">
+        <v>6</v>
+      </c>
+      <c r="D155" s="2">
+        <v>8500</v>
+      </c>
+      <c r="E155" s="2">
+        <f t="shared" si="1"/>
+        <v>8925</v>
+      </c>
+      <c r="G155">
+        <v>8</v>
+      </c>
+      <c r="H155">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>155</v>
+      </c>
+      <c r="B156" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C156" t="s">
+        <v>6</v>
+      </c>
+      <c r="D156" s="2">
+        <v>7000</v>
+      </c>
+      <c r="E156" s="2">
+        <f t="shared" si="1"/>
+        <v>7350</v>
+      </c>
+      <c r="G156">
+        <v>9</v>
+      </c>
+      <c r="H156">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>156</v>
+      </c>
+      <c r="B157" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C157" t="s">
+        <v>6</v>
+      </c>
+      <c r="D157" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E157" s="2">
+        <f t="shared" si="1"/>
+        <v>5250</v>
+      </c>
+      <c r="G157">
+        <v>10</v>
+      </c>
+      <c r="H157">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>157</v>
+      </c>
+      <c r="B158" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C158" t="s">
+        <v>6</v>
+      </c>
+      <c r="D158" s="2">
+        <v>6000</v>
+      </c>
+      <c r="E158" s="2">
+        <f t="shared" si="1"/>
+        <v>6300</v>
+      </c>
+      <c r="G158">
+        <v>11</v>
+      </c>
+      <c r="H158">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>158</v>
+      </c>
+      <c r="B159" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C159" t="s">
+        <v>6</v>
+      </c>
+      <c r="D159" s="2">
+        <v>3050</v>
+      </c>
+      <c r="E159" s="2">
+        <f t="shared" si="1"/>
+        <v>3203</v>
+      </c>
+      <c r="G159">
+        <v>12</v>
+      </c>
+      <c r="H159">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>159</v>
+      </c>
+      <c r="B160" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C160" t="s">
+        <v>6</v>
+      </c>
+      <c r="D160" s="2">
+        <v>11000</v>
+      </c>
+      <c r="E160" s="2">
+        <f t="shared" si="1"/>
+        <v>11550</v>
+      </c>
+      <c r="G160">
+        <v>13</v>
+      </c>
+      <c r="H160">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>160</v>
+      </c>
+      <c r="B161" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C161" t="s">
+        <v>6</v>
+      </c>
+      <c r="D161" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E161" s="2">
+        <f t="shared" si="1"/>
+        <v>2100</v>
+      </c>
+      <c r="G161">
+        <v>14</v>
+      </c>
+      <c r="H161">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>161</v>
+      </c>
+      <c r="B162" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C162" t="s">
+        <v>6</v>
+      </c>
+      <c r="D162" s="2">
+        <v>10500</v>
+      </c>
+      <c r="E162" s="2">
+        <f t="shared" si="1"/>
+        <v>11025</v>
+      </c>
+      <c r="G162">
+        <v>15</v>
+      </c>
+      <c r="H162">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>162</v>
+      </c>
+      <c r="B163" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C163" t="s">
+        <v>6</v>
+      </c>
+      <c r="D163" s="2">
+        <v>6500</v>
+      </c>
+      <c r="E163" s="2">
+        <f t="shared" si="1"/>
+        <v>6825</v>
+      </c>
+      <c r="G163">
+        <v>16</v>
+      </c>
+      <c r="H163">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>163</v>
+      </c>
+      <c r="B164" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C164" t="s">
+        <v>6</v>
+      </c>
+      <c r="D164" s="2">
+        <v>4500</v>
+      </c>
+      <c r="E164" s="2">
+        <f t="shared" si="1"/>
+        <v>4725</v>
+      </c>
+      <c r="G164">
+        <v>17</v>
+      </c>
+      <c r="H164">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>164</v>
+      </c>
+      <c r="B165" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C165" t="s">
+        <v>6</v>
+      </c>
+      <c r="D165" s="2">
+        <v>15500</v>
+      </c>
+      <c r="E165" s="2">
+        <f t="shared" si="1"/>
+        <v>16275</v>
+      </c>
+      <c r="G165">
+        <v>18</v>
+      </c>
+      <c r="H165">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>165</v>
+      </c>
+      <c r="B166" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C166" t="s">
+        <v>6</v>
+      </c>
+      <c r="D166" s="2">
+        <v>9500</v>
+      </c>
+      <c r="E166" s="2">
+        <f t="shared" si="1"/>
+        <v>9975</v>
+      </c>
+      <c r="G166">
+        <v>19</v>
+      </c>
+      <c r="H166">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>166</v>
+      </c>
+      <c r="B167" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C167" t="s">
+        <v>6</v>
+      </c>
+      <c r="D167" s="2">
+        <v>9500</v>
+      </c>
+      <c r="E167" s="2">
+        <f t="shared" si="1"/>
+        <v>9975</v>
+      </c>
+      <c r="G167">
+        <v>20</v>
+      </c>
+      <c r="H167">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>167</v>
+      </c>
+      <c r="B168" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C168" t="s">
+        <v>6</v>
+      </c>
+      <c r="D168" s="2">
+        <v>12500</v>
+      </c>
+      <c r="E168" s="2">
+        <f t="shared" si="1"/>
+        <v>13125</v>
+      </c>
+      <c r="G168">
+        <v>21</v>
+      </c>
+      <c r="H168">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>168</v>
+      </c>
+      <c r="B169" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C169" t="s">
+        <v>6</v>
+      </c>
+      <c r="D169" s="2">
+        <v>21000</v>
+      </c>
+      <c r="E169" s="2">
+        <f t="shared" si="1"/>
+        <v>22050</v>
+      </c>
+      <c r="G169">
+        <v>22</v>
+      </c>
+      <c r="H169">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>169</v>
+      </c>
+      <c r="B170" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C170" t="s">
+        <v>6</v>
+      </c>
+      <c r="D170" s="2">
+        <v>19000</v>
+      </c>
+      <c r="E170" s="2">
+        <f t="shared" si="1"/>
+        <v>19950</v>
+      </c>
+      <c r="G170">
+        <v>23</v>
+      </c>
+      <c r="H170">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>170</v>
+      </c>
+      <c r="B171" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C171" t="s">
+        <v>6</v>
+      </c>
+      <c r="D171" s="2">
+        <v>29500</v>
+      </c>
+      <c r="E171" s="2">
+        <f t="shared" si="1"/>
+        <v>30975</v>
+      </c>
+      <c r="G171">
+        <v>24</v>
+      </c>
+      <c r="H171">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>171</v>
+      </c>
+      <c r="B172" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C172" t="s">
+        <v>6</v>
+      </c>
+      <c r="D172" s="2">
+        <v>39500</v>
+      </c>
+      <c r="E172" s="2">
+        <f t="shared" si="1"/>
+        <v>41475</v>
+      </c>
+      <c r="G172">
+        <v>25</v>
+      </c>
+      <c r="H172">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>172</v>
+      </c>
+      <c r="B173" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C173" t="s">
+        <v>6</v>
+      </c>
+      <c r="D173" s="2">
+        <v>12500</v>
+      </c>
+      <c r="E173" s="2">
+        <f t="shared" si="1"/>
+        <v>13125</v>
+      </c>
+      <c r="G173">
+        <v>26</v>
+      </c>
+      <c r="H173">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>173</v>
+      </c>
+      <c r="B174" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C174" t="s">
+        <v>6</v>
+      </c>
+      <c r="D174" s="2">
+        <v>20500</v>
+      </c>
+      <c r="E174" s="2">
+        <f t="shared" si="1"/>
+        <v>21525</v>
+      </c>
+      <c r="G174">
+        <v>27</v>
+      </c>
+      <c r="H174">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>174</v>
+      </c>
+      <c r="B175" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C175" t="s">
+        <v>6</v>
+      </c>
+      <c r="D175" s="2">
+        <v>5500</v>
+      </c>
+      <c r="E175" s="2">
+        <f t="shared" si="1"/>
+        <v>5775</v>
+      </c>
+      <c r="G175">
+        <v>28</v>
+      </c>
+      <c r="H175">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>175</v>
+      </c>
+      <c r="B176" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C176" t="s">
+        <v>6</v>
+      </c>
+      <c r="D176" s="2">
+        <v>6500</v>
+      </c>
+      <c r="E176" s="2">
+        <f t="shared" si="1"/>
+        <v>6825</v>
+      </c>
+      <c r="G176">
+        <v>29</v>
+      </c>
+      <c r="H176">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>176</v>
+      </c>
+      <c r="B177" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C177" t="s">
+        <v>6</v>
+      </c>
+      <c r="D177" s="2">
+        <v>4000</v>
+      </c>
+      <c r="E177" s="2">
+        <f t="shared" si="1"/>
+        <v>4200</v>
+      </c>
+      <c r="G177">
+        <v>30</v>
+      </c>
+      <c r="H177">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>177</v>
+      </c>
+      <c r="B178" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C178" t="s">
+        <v>6</v>
+      </c>
+      <c r="D178" s="2">
+        <v>3000</v>
+      </c>
+      <c r="E178" s="2">
+        <f t="shared" si="1"/>
+        <v>3150</v>
+      </c>
+      <c r="G178">
+        <v>31</v>
+      </c>
+      <c r="H178">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>178</v>
+      </c>
+      <c r="B179" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C179" t="s">
+        <v>6</v>
+      </c>
+      <c r="D179" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E179" s="2">
+        <f t="shared" si="1"/>
+        <v>2100</v>
+      </c>
+      <c r="G179">
+        <v>32</v>
+      </c>
+      <c r="H179">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>179</v>
+      </c>
+      <c r="B180" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C180" t="s">
+        <v>6</v>
+      </c>
+      <c r="D180" s="2">
+        <v>1500</v>
+      </c>
+      <c r="E180" s="2">
+        <f t="shared" si="1"/>
+        <v>1575</v>
+      </c>
+      <c r="G180">
+        <v>33</v>
+      </c>
+      <c r="H180">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>180</v>
+      </c>
+      <c r="B181" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C181" t="s">
+        <v>6</v>
+      </c>
+      <c r="D181" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E181" s="2">
+        <f t="shared" si="1"/>
+        <v>2100</v>
+      </c>
+      <c r="G181">
+        <v>34</v>
+      </c>
+      <c r="H181">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>181</v>
+      </c>
+      <c r="B182" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C182" t="s">
+        <v>6</v>
+      </c>
+      <c r="D182" s="2">
+        <v>3000</v>
+      </c>
+      <c r="E182" s="2">
+        <f t="shared" si="1"/>
+        <v>3150</v>
+      </c>
+      <c r="G182">
+        <v>35</v>
+      </c>
+      <c r="H182">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>182</v>
+      </c>
+      <c r="B183" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C183" t="s">
+        <v>6</v>
+      </c>
+      <c r="D183" s="2">
+        <v>1500</v>
+      </c>
+      <c r="E183" s="2">
+        <f t="shared" ref="E183:E220" si="2">ROUND(D183+5%*D183,0)</f>
+        <v>1575</v>
+      </c>
+      <c r="G183">
+        <v>36</v>
+      </c>
+      <c r="H183">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>183</v>
+      </c>
+      <c r="B184" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C184" t="s">
+        <v>6</v>
+      </c>
+      <c r="D184" s="2">
+        <v>3000</v>
+      </c>
+      <c r="E184" s="2">
+        <f t="shared" si="2"/>
+        <v>3150</v>
+      </c>
+      <c r="G184">
+        <v>37</v>
+      </c>
+      <c r="H184">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>184</v>
+      </c>
+      <c r="B185" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C185" t="s">
+        <v>6</v>
+      </c>
+      <c r="D185" s="2">
+        <v>9000</v>
+      </c>
+      <c r="E185" s="2">
+        <f t="shared" si="2"/>
+        <v>9450</v>
+      </c>
+      <c r="G185">
+        <v>38</v>
+      </c>
+      <c r="H185">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>185</v>
+      </c>
+      <c r="B186" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C186" t="s">
+        <v>6</v>
+      </c>
+      <c r="D186" s="2">
+        <v>2500</v>
+      </c>
+      <c r="E186" s="2">
+        <f t="shared" si="2"/>
+        <v>2625</v>
+      </c>
+      <c r="G186">
+        <v>39</v>
+      </c>
+      <c r="H186">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>186</v>
+      </c>
+      <c r="B187" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C187" t="s">
+        <v>6</v>
+      </c>
+      <c r="D187" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E187" s="2">
+        <f t="shared" si="2"/>
+        <v>2100</v>
+      </c>
+      <c r="G187">
+        <v>40</v>
+      </c>
+      <c r="H187">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>187</v>
+      </c>
+      <c r="B188" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C188" t="s">
+        <v>6</v>
+      </c>
+      <c r="D188" s="2">
+        <v>1500</v>
+      </c>
+      <c r="E188" s="2">
+        <f t="shared" si="2"/>
+        <v>1575</v>
+      </c>
+      <c r="G188">
+        <v>41</v>
+      </c>
+      <c r="H188">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>188</v>
+      </c>
+      <c r="B189" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C189" t="s">
+        <v>6</v>
+      </c>
+      <c r="D189" s="2">
+        <v>3500</v>
+      </c>
+      <c r="E189" s="2">
+        <f t="shared" si="2"/>
+        <v>3675</v>
+      </c>
+      <c r="G189">
+        <v>42</v>
+      </c>
+      <c r="H189">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>189</v>
+      </c>
+      <c r="B190" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C190" t="s">
+        <v>6</v>
+      </c>
+      <c r="D190" s="2">
+        <v>3000</v>
+      </c>
+      <c r="E190" s="2">
+        <f t="shared" si="2"/>
+        <v>3150</v>
+      </c>
+      <c r="G190">
+        <v>43</v>
+      </c>
+      <c r="H190">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>190</v>
+      </c>
+      <c r="B191" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C191" t="s">
+        <v>6</v>
+      </c>
+      <c r="D191" s="2">
+        <v>2500</v>
+      </c>
+      <c r="E191" s="2">
+        <f t="shared" si="2"/>
+        <v>2625</v>
+      </c>
+      <c r="G191">
+        <v>44</v>
+      </c>
+      <c r="H191">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>191</v>
+      </c>
+      <c r="B192" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C192" t="s">
+        <v>6</v>
+      </c>
+      <c r="D192" s="2">
+        <v>4000</v>
+      </c>
+      <c r="E192" s="2">
+        <f t="shared" si="2"/>
+        <v>4200</v>
+      </c>
+      <c r="G192">
+        <v>45</v>
+      </c>
+      <c r="H192">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>192</v>
+      </c>
+      <c r="B193" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C193" t="s">
+        <v>6</v>
+      </c>
+      <c r="D193" s="2">
+        <v>750</v>
+      </c>
+      <c r="E193" s="2">
+        <f t="shared" si="2"/>
+        <v>788</v>
+      </c>
+      <c r="G193">
+        <v>46</v>
+      </c>
+      <c r="H193">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>193</v>
+      </c>
+      <c r="B194" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C194" t="s">
+        <v>6</v>
+      </c>
+      <c r="D194" s="2">
+        <v>0</v>
+      </c>
+      <c r="E194" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G194">
+        <v>47</v>
+      </c>
+      <c r="H194">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>194</v>
+      </c>
+      <c r="B195" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C195" t="s">
+        <v>6</v>
+      </c>
+      <c r="D195" s="2">
+        <v>11000</v>
+      </c>
+      <c r="E195" s="2">
         <f t="shared" si="2"/>
         <v>11550</v>
       </c>
-      <c r="G145">
+      <c r="G195">
         <v>48</v>
       </c>
-      <c r="H145">
+      <c r="H195">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>195</v>
+      </c>
+      <c r="B196" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C196" t="s">
+        <v>6</v>
+      </c>
+      <c r="D196" s="2">
+        <v>0</v>
+      </c>
+      <c r="E196" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G196">
+        <v>49</v>
+      </c>
+      <c r="H196">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>196</v>
+      </c>
+      <c r="B197" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C197" t="s">
+        <v>6</v>
+      </c>
+      <c r="D197" s="2">
+        <v>0</v>
+      </c>
+      <c r="E197" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G197">
+        <v>50</v>
+      </c>
+      <c r="H197">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>197</v>
+      </c>
+      <c r="B198" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C198" t="s">
+        <v>6</v>
+      </c>
+      <c r="D198" s="2">
+        <v>0</v>
+      </c>
+      <c r="E198" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G198">
+        <v>51</v>
+      </c>
+      <c r="H198">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>198</v>
+      </c>
+      <c r="B199" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C199" t="s">
+        <v>6</v>
+      </c>
+      <c r="D199" s="2">
+        <v>0</v>
+      </c>
+      <c r="E199" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G199">
+        <v>52</v>
+      </c>
+      <c r="H199">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>199</v>
+      </c>
+      <c r="B200" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C200" t="s">
+        <v>6</v>
+      </c>
+      <c r="D200" s="2">
+        <v>0</v>
+      </c>
+      <c r="E200" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G200">
+        <v>53</v>
+      </c>
+      <c r="H200">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>200</v>
+      </c>
+      <c r="B201" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C201" t="s">
+        <v>6</v>
+      </c>
+      <c r="D201" s="2">
+        <v>9000</v>
+      </c>
+      <c r="E201" s="2">
+        <f t="shared" si="2"/>
+        <v>9450</v>
+      </c>
+      <c r="G201">
+        <v>54</v>
+      </c>
+      <c r="H201">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>201</v>
+      </c>
+      <c r="B202" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C202" t="s">
+        <v>6</v>
+      </c>
+      <c r="D202" s="2">
+        <v>2500</v>
+      </c>
+      <c r="E202" s="2">
+        <f t="shared" si="2"/>
+        <v>2625</v>
+      </c>
+      <c r="G202">
+        <v>55</v>
+      </c>
+      <c r="H202">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>202</v>
+      </c>
+      <c r="B203" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C203" t="s">
+        <v>6</v>
+      </c>
+      <c r="D203" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E203" s="2">
+        <f t="shared" si="2"/>
+        <v>2100</v>
+      </c>
+      <c r="G203">
+        <v>56</v>
+      </c>
+      <c r="H203">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>203</v>
+      </c>
+      <c r="B204" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C204" t="s">
+        <v>6</v>
+      </c>
+      <c r="D204" s="2">
+        <v>1500</v>
+      </c>
+      <c r="E204" s="2">
+        <f t="shared" si="2"/>
+        <v>1575</v>
+      </c>
+      <c r="G204">
+        <v>57</v>
+      </c>
+      <c r="H204">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>204</v>
+      </c>
+      <c r="B205" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C205" t="s">
+        <v>6</v>
+      </c>
+      <c r="D205" s="2">
+        <v>3500</v>
+      </c>
+      <c r="E205" s="2">
+        <f t="shared" si="2"/>
+        <v>3675</v>
+      </c>
+      <c r="G205">
+        <v>58</v>
+      </c>
+      <c r="H205">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>205</v>
+      </c>
+      <c r="B206" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C206" t="s">
+        <v>6</v>
+      </c>
+      <c r="D206" s="2">
+        <v>3000</v>
+      </c>
+      <c r="E206" s="2">
+        <f t="shared" si="2"/>
+        <v>3150</v>
+      </c>
+      <c r="G206">
+        <v>59</v>
+      </c>
+      <c r="H206">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>206</v>
+      </c>
+      <c r="B207" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C207" t="s">
+        <v>6</v>
+      </c>
+      <c r="D207" s="2">
+        <v>2500</v>
+      </c>
+      <c r="E207" s="2">
+        <f t="shared" si="2"/>
+        <v>2625</v>
+      </c>
+      <c r="G207">
+        <v>60</v>
+      </c>
+      <c r="H207">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>207</v>
+      </c>
+      <c r="B208" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C208" t="s">
+        <v>6</v>
+      </c>
+      <c r="D208" s="2">
+        <v>4000</v>
+      </c>
+      <c r="E208" s="2">
+        <f t="shared" si="2"/>
+        <v>4200</v>
+      </c>
+      <c r="G208">
+        <v>61</v>
+      </c>
+      <c r="H208">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>208</v>
+      </c>
+      <c r="B209" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C209" t="s">
+        <v>6</v>
+      </c>
+      <c r="D209" s="2">
+        <v>750</v>
+      </c>
+      <c r="E209" s="2">
+        <f t="shared" si="2"/>
+        <v>788</v>
+      </c>
+      <c r="G209">
+        <v>62</v>
+      </c>
+      <c r="H209">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>209</v>
+      </c>
+      <c r="B210" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C210" t="s">
+        <v>6</v>
+      </c>
+      <c r="D210" s="2">
+        <v>3000</v>
+      </c>
+      <c r="E210" s="2">
+        <f t="shared" si="2"/>
+        <v>3150</v>
+      </c>
+      <c r="G210">
+        <v>63</v>
+      </c>
+      <c r="H210">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>210</v>
+      </c>
+      <c r="B211" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C211" t="s">
+        <v>6</v>
+      </c>
+      <c r="D211" s="2">
+        <v>11000</v>
+      </c>
+      <c r="E211" s="2">
+        <f t="shared" si="2"/>
+        <v>11550</v>
+      </c>
+      <c r="G211">
+        <v>64</v>
+      </c>
+      <c r="H211">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>211</v>
+      </c>
+      <c r="B212" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C212" t="s">
+        <v>6</v>
+      </c>
+      <c r="D212" s="2">
+        <v>0</v>
+      </c>
+      <c r="E212" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G212">
+        <v>65</v>
+      </c>
+      <c r="H212">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>212</v>
+      </c>
+      <c r="B213" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C213" t="s">
+        <v>6</v>
+      </c>
+      <c r="D213" s="2">
+        <v>3500</v>
+      </c>
+      <c r="E213" s="2">
+        <f t="shared" si="2"/>
+        <v>3675</v>
+      </c>
+      <c r="G213">
+        <v>66</v>
+      </c>
+      <c r="H213">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>213</v>
+      </c>
+      <c r="B214" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C214" t="s">
+        <v>6</v>
+      </c>
+      <c r="D214" s="2">
+        <v>1500</v>
+      </c>
+      <c r="E214" s="2">
+        <f t="shared" si="2"/>
+        <v>1575</v>
+      </c>
+      <c r="G214">
+        <v>67</v>
+      </c>
+      <c r="H214">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>214</v>
+      </c>
+      <c r="B215" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C215" t="s">
+        <v>6</v>
+      </c>
+      <c r="D215" s="2">
+        <v>1500</v>
+      </c>
+      <c r="E215" s="2">
+        <f t="shared" si="2"/>
+        <v>1575</v>
+      </c>
+      <c r="G215">
+        <v>68</v>
+      </c>
+      <c r="H215">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>215</v>
+      </c>
+      <c r="B216" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C216" t="s">
+        <v>6</v>
+      </c>
+      <c r="D216" s="2">
+        <v>2500</v>
+      </c>
+      <c r="E216" s="2">
+        <f t="shared" si="2"/>
+        <v>2625</v>
+      </c>
+      <c r="G216">
+        <v>69</v>
+      </c>
+      <c r="H216">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>216</v>
+      </c>
+      <c r="B217" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C217" t="s">
+        <v>6</v>
+      </c>
+      <c r="D217" s="2">
+        <v>3500</v>
+      </c>
+      <c r="E217" s="2">
+        <f t="shared" si="2"/>
+        <v>3675</v>
+      </c>
+      <c r="G217">
+        <v>70</v>
+      </c>
+      <c r="H217">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>217</v>
+      </c>
+      <c r="B218" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C218" t="s">
+        <v>6</v>
+      </c>
+      <c r="D218" s="2">
+        <v>5500</v>
+      </c>
+      <c r="E218" s="2">
+        <f t="shared" si="2"/>
+        <v>5775</v>
+      </c>
+      <c r="G218">
+        <v>71</v>
+      </c>
+      <c r="H218">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>218</v>
+      </c>
+      <c r="B219" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C219" t="s">
+        <v>6</v>
+      </c>
+      <c r="D219" s="2">
+        <v>3500</v>
+      </c>
+      <c r="E219" s="2">
+        <f t="shared" si="2"/>
+        <v>3675</v>
+      </c>
+      <c r="G219">
+        <v>72</v>
+      </c>
+      <c r="H219">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>219</v>
+      </c>
+      <c r="B220" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C220" t="s">
+        <v>6</v>
+      </c>
+      <c r="D220" s="2">
+        <v>0</v>
+      </c>
+      <c r="E220" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G220">
+        <v>73</v>
+      </c>
+      <c r="H220">
         <v>3</v>
       </c>
     </row>
@@ -4272,8 +6072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50:E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Menghapus `Bahan` dan menggabungkannya ke dalam `Kategori`.
</commit_message>
<xml_diff>
--- a/data_awal.xlsx
+++ b/data_awal.xlsx
@@ -4,23 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="hibernate_sequences" sheetId="2" r:id="rId1"/>
     <sheet name="work" sheetId="3" r:id="rId2"/>
     <sheet name="itempakaian" sheetId="1" r:id="rId3"/>
     <sheet name="kategori" sheetId="4" r:id="rId4"/>
-    <sheet name="bahan" sheetId="7" r:id="rId5"/>
-    <sheet name="jeniswork" sheetId="5" r:id="rId6"/>
-    <sheet name="pelanggan" sheetId="6" r:id="rId7"/>
+    <sheet name="jeniswork" sheetId="5" r:id="rId5"/>
+    <sheet name="pelanggan" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="115">
   <si>
     <t>id</t>
   </si>
@@ -767,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A220"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7359,10 +7358,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7446,6 +7445,23 @@
         <v>64</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>41643.677465277775</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" t="s">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7453,87 +7469,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>41643.677407407406</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>41643.677465277775</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -7623,7 +7561,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>

</xml_diff>